<commit_message>
Add a read me file
</commit_message>
<xml_diff>
--- a/data/18650/18605_-10_dc_1.xlsx
+++ b/data/18650/18605_-10_dc_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane\Desktop\Battery_lowtemperature\pythonProject\data\18650\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439757AD-4E0A-42A2-B0F6-1B9FBBCA3B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92C94B1-21C5-4BCF-AFD2-0E8BD80B6EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -373,8 +373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F321"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
+      <selection activeCell="J298" sqref="J298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -438,12 +438,12 @@
         <v>-3.3948900000000002</v>
       </c>
       <c r="E3">
-        <f>E2+((A3/3600)*D3)</f>
-        <v>3014.9905697499998</v>
+        <f>E2+((10/3600)*D3*1000)</f>
+        <v>3005.5697500000001</v>
       </c>
       <c r="F3">
         <f>E3/3400</f>
-        <v>0.88676193227941169</v>
+        <v>0.88399110294117655</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -460,12 +460,12 @@
         <v>-3.3947699999999998</v>
       </c>
       <c r="E4">
-        <f>E3+((A4/3600)*D4)</f>
-        <v>3014.9717099166664</v>
+        <f>E3+((10/3600)*D4*1000)</f>
+        <v>2996.1398333333336</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F66" si="0">E4/3400</f>
-        <v>0.88675638526960776</v>
+        <f>E4/3400</f>
+        <v>0.88121759803921573</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -482,12 +482,12 @@
         <v>-3.3948700000000001</v>
       </c>
       <c r="E5">
-        <f>E4+((A5/3600)*D5)</f>
-        <v>3014.9434193333332</v>
+        <f t="shared" ref="E5:E68" si="0">E4+((10/3600)*D5*1000)</f>
+        <v>2986.709638888889</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
-        <v>0.88674806450980392</v>
+        <f t="shared" ref="F4:F66" si="1">E5/3400</f>
+        <v>0.87844401143790851</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -504,12 +504,12 @@
         <v>-3.3949199999999999</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E68" si="1">E5+((A6/3600)*D6)</f>
-        <v>3014.905698</v>
+        <f t="shared" si="0"/>
+        <v>2977.2793055555558</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
-        <v>0.88673696999999996</v>
+        <f t="shared" si="1"/>
+        <v>0.8756703839869282</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -526,12 +526,12 @@
         <v>-3.3948900000000002</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
-        <v>3014.8585467500002</v>
+        <f t="shared" si="0"/>
+        <v>2967.8490555555559</v>
       </c>
       <c r="F7">
         <f>E7/3400</f>
-        <v>0.88672310198529414</v>
+        <v>0.87289678104575175</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -548,12 +548,12 @@
         <v>-3.3946999999999998</v>
       </c>
       <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2958.4193333333337</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="1"/>
-        <v>3014.801968416667</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0.88670646129901975</v>
+        <v>0.87012333333333347</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -570,12 +570,12 @@
         <v>-3.3949199999999999</v>
       </c>
       <c r="E9">
+        <f t="shared" si="0"/>
+        <v>2948.9890000000005</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="1"/>
-        <v>3014.7359560833338</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0.88668704590686287</v>
+        <v>0.86734970588235305</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -592,12 +592,12 @@
         <v>-3.3947400000000001</v>
       </c>
       <c r="E10">
+        <f t="shared" si="0"/>
+        <v>2939.5591666666674</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="1"/>
-        <v>3014.6605174166671</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0.88666485806372564</v>
+        <v>0.8645762254901963</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -614,12 +614,12 @@
         <v>-3.3946499999999999</v>
       </c>
       <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2930.1295833333338</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="1"/>
-        <v>3014.5756511666673</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0.88663989740196092</v>
+        <v>0.86180281862745112</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -636,12 +636,12 @@
         <v>-3.3948700000000001</v>
       </c>
       <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2920.6993888888892</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="1"/>
-        <v>3014.4813492222229</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0.88661216153594791</v>
+        <v>0.8590292320261439</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -658,12 +658,12 @@
         <v>-3.3951799999999999</v>
       </c>
       <c r="E13">
+        <f t="shared" si="0"/>
+        <v>2911.2683333333334</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="1"/>
-        <v>3014.3776076111117</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0.88658164929738581</v>
+        <v>0.85625539215686275</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -680,12 +680,12 @@
         <v>-3.3949099999999999</v>
       </c>
       <c r="E14">
+        <f t="shared" si="0"/>
+        <v>2901.8380277777778</v>
+      </c>
+      <c r="F14">
         <f t="shared" si="1"/>
-        <v>3014.2644439444448</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0.88654836586601315</v>
+        <v>0.85348177287581706</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -702,12 +702,12 @@
         <v>-3.39506</v>
       </c>
       <c r="E15">
+        <f t="shared" si="0"/>
+        <v>2892.4073055555555</v>
+      </c>
+      <c r="F15">
         <f t="shared" si="1"/>
-        <v>3014.141844555556</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0.8865123072222223</v>
+        <v>0.85070803104575166</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -724,12 +724,12 @@
         <v>-3.39507</v>
       </c>
       <c r="E16">
+        <f t="shared" si="0"/>
+        <v>2882.9765555555555</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="1"/>
-        <v>3014.009814055556</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>0.88647347472222238</v>
+        <v>0.84793428104575164</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -746,12 +746,12 @@
         <v>-3.3949199999999999</v>
       </c>
       <c r="E17">
+        <f t="shared" si="0"/>
+        <v>2873.5462222222222</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="1"/>
-        <v>3013.8683590555561</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>0.88643187031045767</v>
+        <v>0.84516065359477122</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -768,12 +768,12 @@
         <v>-3.3946800000000001</v>
       </c>
       <c r="E18">
+        <f t="shared" si="0"/>
+        <v>2864.1165555555554</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="1"/>
-        <v>3013.7174843888893</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>0.88638749540849682</v>
+        <v>0.84238722222222218</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -790,12 +790,12 @@
         <v>-3.3948100000000001</v>
       </c>
       <c r="E19">
+        <f t="shared" si="0"/>
+        <v>2854.6865277777774</v>
+      </c>
+      <c r="F19">
         <f t="shared" si="1"/>
-        <v>3013.5571739166671</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>0.88634034526960803</v>
+        <v>0.83961368464052277</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -812,12 +812,12 @@
         <v>-3.3948299999999998</v>
       </c>
       <c r="E20">
+        <f t="shared" si="0"/>
+        <v>2845.2564444444442</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="1"/>
-        <v>3013.3874324166673</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>0.8862904212990198</v>
+        <v>0.83684013071895413</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -834,12 +834,12 @@
         <v>-3.39506</v>
       </c>
       <c r="E21">
+        <f t="shared" si="0"/>
+        <v>2835.8257222222219</v>
+      </c>
+      <c r="F21">
         <f t="shared" si="1"/>
-        <v>3013.208248694445</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>0.88623772020424851</v>
+        <v>0.83406638888888884</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -856,12 +856,12 @@
         <v>-3.39486</v>
       </c>
       <c r="E22">
+        <f t="shared" si="0"/>
+        <v>2826.3955555555553</v>
+      </c>
+      <c r="F22">
         <f t="shared" si="1"/>
-        <v>3013.0196453611115</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>0.88618224863562101</v>
+        <v>0.83129281045751624</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -878,12 +878,12 @@
         <v>-3.3948299999999998</v>
       </c>
       <c r="E23">
+        <f t="shared" si="0"/>
+        <v>2816.9654722222222</v>
+      </c>
+      <c r="F23">
         <f t="shared" si="1"/>
-        <v>3012.8216136111114</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>0.88612400400326807</v>
+        <v>0.82851925653594771</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -900,12 +900,12 @@
         <v>-3.39506</v>
       </c>
       <c r="E24">
+        <f t="shared" si="0"/>
+        <v>2807.5347499999998</v>
+      </c>
+      <c r="F24">
         <f t="shared" si="1"/>
-        <v>3012.6141377222225</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>0.88606298168300657</v>
+        <v>0.82574551470588231</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -922,12 +922,12 @@
         <v>-3.39486</v>
       </c>
       <c r="E25">
+        <f t="shared" si="0"/>
+        <v>2798.1045833333333</v>
+      </c>
+      <c r="F25">
         <f t="shared" si="1"/>
-        <v>3012.3972438888891</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>0.88599918937908506</v>
+        <v>0.82297193627450982</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -944,12 +944,12 @@
         <v>-3.3946700000000001</v>
       </c>
       <c r="E26">
+        <f t="shared" si="0"/>
+        <v>2788.6749444444445</v>
+      </c>
+      <c r="F26">
         <f t="shared" si="1"/>
-        <v>3012.1709325555557</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="0"/>
-        <v>0.88593262722222232</v>
+        <v>0.8201985130718954</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -966,12 +966,12 @@
         <v>-3.39506</v>
       </c>
       <c r="E27">
+        <f t="shared" si="0"/>
+        <v>2779.2442222222221</v>
+      </c>
+      <c r="F27">
         <f t="shared" si="1"/>
-        <v>3011.9351645000002</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="0"/>
-        <v>0.8858632836764706</v>
+        <v>0.81742477124182999</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -988,12 +988,12 @@
         <v>-3.3947600000000002</v>
       </c>
       <c r="E28">
+        <f t="shared" si="0"/>
+        <v>2769.8143333333333</v>
+      </c>
+      <c r="F28">
         <f t="shared" si="1"/>
-        <v>3011.6899873888892</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="0"/>
-        <v>0.88579117276143804</v>
+        <v>0.8146512745098039</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -1010,12 +1010,12 @@
         <v>-3.3948499999999999</v>
       </c>
       <c r="E29">
+        <f t="shared" si="0"/>
+        <v>2760.3841944444443</v>
+      </c>
+      <c r="F29">
         <f t="shared" si="1"/>
-        <v>3011.4353736388894</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="0"/>
-        <v>0.88571628636437927</v>
+        <v>0.81187770424836603</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1032,12 +1032,12 @@
         <v>-3.3947699999999998</v>
       </c>
       <c r="E30">
+        <f t="shared" si="0"/>
+        <v>2750.9542777777779</v>
+      </c>
+      <c r="F30">
         <f t="shared" si="1"/>
-        <v>3011.1713359722226</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="0"/>
-        <v>0.88563862822712425</v>
+        <v>0.80910419934640521</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1054,12 +1054,12 @@
         <v>-3.3948100000000001</v>
       </c>
       <c r="E31">
+        <f t="shared" si="0"/>
+        <v>2741.5242499999999</v>
+      </c>
+      <c r="F31">
         <f t="shared" si="1"/>
-        <v>3010.8978651666671</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="0"/>
-        <v>0.88555819563725502</v>
+        <v>0.80633066176470591</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1076,12 +1076,12 @@
         <v>-3.39479</v>
       </c>
       <c r="E32">
+        <f t="shared" si="0"/>
+        <v>2732.0942777777777</v>
+      </c>
+      <c r="F32">
         <f t="shared" si="1"/>
-        <v>3010.6149660000005</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="0"/>
-        <v>0.88547499000000018</v>
+        <v>0.80355714052287586</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1098,12 +1098,12 @@
         <v>-3.3949600000000002</v>
       </c>
       <c r="E33">
+        <f t="shared" si="0"/>
+        <v>2722.6638333333335</v>
+      </c>
+      <c r="F33">
         <f t="shared" si="1"/>
-        <v>3010.3226222222229</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="0"/>
-        <v>0.88538900653594788</v>
+        <v>0.80078348039215697</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1120,12 +1120,12 @@
         <v>-3.3948800000000001</v>
       </c>
       <c r="E34">
+        <f t="shared" si="0"/>
+        <v>2713.2336111111113</v>
+      </c>
+      <c r="F34">
         <f t="shared" si="1"/>
-        <v>3010.0208551111118</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="0"/>
-        <v>0.88530025150326819</v>
+        <v>0.79800988562091513</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -1142,12 +1142,12 @@
         <v>-3.3949500000000001</v>
       </c>
       <c r="E35">
+        <f t="shared" si="0"/>
+        <v>2703.8031944444447</v>
+      </c>
+      <c r="F35">
         <f t="shared" si="1"/>
-        <v>3009.7096513611118</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="0"/>
-        <v>0.88520872098856229</v>
+        <v>0.79523623366013074</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -1164,12 +1164,12 @@
         <v>-3.3949600000000002</v>
       </c>
       <c r="E36">
+        <f t="shared" si="0"/>
+        <v>2694.3727500000005</v>
+      </c>
+      <c r="F36">
         <f t="shared" si="1"/>
-        <v>3009.3890162500006</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="0"/>
-        <v>0.88511441654411782</v>
+        <v>0.79246257352941185</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1186,12 +1186,12 @@
         <v>-3.3948399999999999</v>
       </c>
       <c r="E37">
+        <f t="shared" si="0"/>
+        <v>2684.9426388888892</v>
+      </c>
+      <c r="F37">
         <f t="shared" si="1"/>
-        <v>3009.0589623611118</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="0"/>
-        <v>0.88501734187091519</v>
+        <v>0.78968901143790859</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1208,12 +1208,12 @@
         <v>-3.3947099999999999</v>
       </c>
       <c r="E38">
+        <f t="shared" si="0"/>
+        <v>2675.5128888888894</v>
+      </c>
+      <c r="F38">
         <f t="shared" si="1"/>
-        <v>3008.719491361112</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="0"/>
-        <v>0.8849174974591506</v>
+        <v>0.7869155555555557</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1230,12 +1230,12 @@
         <v>-3.3949600000000002</v>
       </c>
       <c r="E39">
+        <f t="shared" si="0"/>
+        <v>2666.0824444444452</v>
+      </c>
+      <c r="F39">
         <f t="shared" si="1"/>
-        <v>3008.3705649166677</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="0"/>
-        <v>0.88481487203431408</v>
+        <v>0.78414189542483681</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -1252,12 +1252,12 @@
         <v>-3.39493</v>
       </c>
       <c r="E40">
+        <f t="shared" si="0"/>
+        <v>2656.6520833333338</v>
+      </c>
+      <c r="F40">
         <f t="shared" si="1"/>
-        <v>3008.0122111944456</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="0"/>
-        <v>0.8847094738807193</v>
+        <v>0.78136825980392177</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -1274,12 +1274,12 @@
         <v>-3.3948800000000001</v>
       </c>
       <c r="E41">
+        <f t="shared" si="0"/>
+        <v>2647.2218611111116</v>
+      </c>
+      <c r="F41">
         <f t="shared" si="1"/>
-        <v>3007.6444325277789</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="0"/>
-        <v>0.88460130368464085</v>
+        <v>0.77859466503267993</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -1296,12 +1296,12 @@
         <v>-3.3950100000000001</v>
       </c>
       <c r="E42">
+        <f t="shared" si="0"/>
+        <v>2637.7912777777783</v>
+      </c>
+      <c r="F42">
         <f t="shared" si="1"/>
-        <v>3007.2672091944455</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="0"/>
-        <v>0.88449035564542511</v>
+        <v>0.77582096405228773</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1318,12 +1318,12 @@
         <v>-3.3946299999999998</v>
       </c>
       <c r="E43">
+        <f t="shared" si="0"/>
+        <v>2628.3617500000005</v>
+      </c>
+      <c r="F43">
         <f t="shared" si="1"/>
-        <v>3006.8805985555568</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="0"/>
-        <v>0.8843766466339873</v>
+        <v>0.77304757352941189</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -1340,12 +1340,12 @@
         <v>-3.39486</v>
       </c>
       <c r="E44">
+        <f t="shared" si="0"/>
+        <v>2618.9315833333339</v>
+      </c>
+      <c r="F44">
         <f t="shared" si="1"/>
-        <v>3006.4845315555567</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="0"/>
-        <v>0.88426015633986965</v>
+        <v>0.7702739950980394</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -1362,12 +1362,12 @@
         <v>-3.3948200000000002</v>
       </c>
       <c r="E45">
+        <f t="shared" si="0"/>
+        <v>2609.5015277777784</v>
+      </c>
+      <c r="F45">
         <f t="shared" si="1"/>
-        <v>3006.0790391666678</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="0"/>
-        <v>0.88414089387254935</v>
+        <v>0.76750044934640538</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -1384,12 +1384,12 @@
         <v>-3.3949500000000001</v>
       </c>
       <c r="E46">
+        <f t="shared" si="0"/>
+        <v>2600.0711111111118</v>
+      </c>
+      <c r="F46">
         <f t="shared" si="1"/>
-        <v>3005.6641008333345</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="0"/>
-        <v>0.88401885318627482</v>
+        <v>0.7647267973856211</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -1406,12 +1406,12 @@
         <v>-3.39507</v>
       </c>
       <c r="E47">
+        <f t="shared" si="0"/>
+        <v>2590.6403611111118</v>
+      </c>
+      <c r="F47">
         <f t="shared" si="1"/>
-        <v>3005.2397170833347</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="0"/>
-        <v>0.8838940344362749</v>
+        <v>0.76195304738562109</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -1428,12 +1428,12 @@
         <v>-3.3947699999999998</v>
       </c>
       <c r="E48">
+        <f t="shared" si="0"/>
+        <v>2581.2104444444453</v>
+      </c>
+      <c r="F48">
         <f t="shared" si="1"/>
-        <v>3004.8059409166681</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="0"/>
-        <v>0.88376645321078473</v>
+        <v>0.75917954248366037</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -1450,12 +1450,12 @@
         <v>-3.3948200000000002</v>
       </c>
       <c r="E49">
+        <f t="shared" si="0"/>
+        <v>2571.7803888888898</v>
+      </c>
+      <c r="F49">
         <f t="shared" si="1"/>
-        <v>3004.3627283055571</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="0"/>
-        <v>0.88363609656045794</v>
+        <v>0.75640599673202635</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -1472,12 +1472,12 @@
         <v>-3.3948399999999999</v>
       </c>
       <c r="E50">
+        <f t="shared" si="0"/>
+        <v>2562.3502777777785</v>
+      </c>
+      <c r="F50">
         <f t="shared" si="1"/>
-        <v>3003.9100829722238</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="0"/>
-        <v>0.8835029655800658</v>
+        <v>0.7536324346405231</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -1494,12 +1494,12 @@
         <v>-3.39506</v>
       </c>
       <c r="E51">
+        <f t="shared" si="0"/>
+        <v>2552.9195555555561</v>
+      </c>
+      <c r="F51">
         <f t="shared" si="1"/>
-        <v>3003.4479775833347</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="0"/>
-        <v>0.88336705223039258</v>
+        <v>0.7508586928104577</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -1516,12 +1516,12 @@
         <v>-3.3946999999999998</v>
       </c>
       <c r="E52">
+        <f t="shared" si="0"/>
+        <v>2543.489833333334</v>
+      </c>
+      <c r="F52">
         <f t="shared" si="1"/>
-        <v>3002.9764914722236</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="0"/>
-        <v>0.88322837984477165</v>
+        <v>0.74808524509803942</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -1538,12 +1538,12 @@
         <v>-3.3946299999999998</v>
       </c>
       <c r="E53">
+        <f t="shared" si="0"/>
+        <v>2534.0603055555562</v>
+      </c>
+      <c r="F53">
         <f t="shared" si="1"/>
-        <v>3002.4955855555568</v>
-      </c>
-      <c r="F53">
-        <f t="shared" si="0"/>
-        <v>0.88308693692810492</v>
+        <v>0.74531185457516358</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -1560,12 +1560,12 @@
         <v>-3.3948200000000002</v>
       </c>
       <c r="E54">
+        <f t="shared" si="0"/>
+        <v>2524.6302500000006</v>
+      </c>
+      <c r="F54">
         <f t="shared" si="1"/>
-        <v>3002.005222666668</v>
-      </c>
-      <c r="F54">
-        <f t="shared" si="0"/>
-        <v>0.88294271254902001</v>
+        <v>0.74253830882352956</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -1582,12 +1582,12 @@
         <v>-3.39486</v>
       </c>
       <c r="E55">
+        <f t="shared" si="0"/>
+        <v>2515.2000833333341</v>
+      </c>
+      <c r="F55">
         <f t="shared" si="1"/>
-        <v>3001.5054238333346</v>
-      </c>
-      <c r="F55">
-        <f t="shared" si="0"/>
-        <v>0.88279571289215719</v>
+        <v>0.73976473039215707</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -1604,12 +1604,12 @@
         <v>-3.39486</v>
       </c>
       <c r="E56">
+        <f t="shared" si="0"/>
+        <v>2505.7699166666675</v>
+      </c>
+      <c r="F56">
         <f t="shared" si="1"/>
-        <v>3000.9961948333348</v>
-      </c>
-      <c r="F56">
-        <f t="shared" si="0"/>
-        <v>0.88264593965686322</v>
+        <v>0.73699115196078457</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -1626,12 +1626,12 @@
         <v>-3.3947699999999998</v>
       </c>
       <c r="E57">
+        <f t="shared" si="0"/>
+        <v>2496.3400000000011</v>
+      </c>
+      <c r="F57">
         <f t="shared" si="1"/>
-        <v>3000.4775494166684</v>
-      </c>
-      <c r="F57">
-        <f t="shared" si="0"/>
-        <v>0.88249339688725537</v>
+        <v>0.73421764705882386</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -1648,12 +1648,12 @@
         <v>-3.3949600000000002</v>
       </c>
       <c r="E58">
+        <f t="shared" si="0"/>
+        <v>2486.9095555555568</v>
+      </c>
+      <c r="F58">
         <f t="shared" si="1"/>
-        <v>2999.9494445277796</v>
-      </c>
-      <c r="F58">
-        <f t="shared" si="0"/>
-        <v>0.88233807191993519</v>
+        <v>0.73144398692810497</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -1670,12 +1670,12 @@
         <v>-3.3948100000000001</v>
       </c>
       <c r="E59">
+        <f t="shared" si="0"/>
+        <v>2477.4795277777789</v>
+      </c>
+      <c r="F59">
         <f t="shared" si="1"/>
-        <v>2999.4119329444461</v>
-      </c>
-      <c r="F59">
-        <f t="shared" si="0"/>
-        <v>0.88217998027777822</v>
+        <v>0.72867044934640557</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -1692,12 +1692,12 @@
         <v>-3.39472</v>
       </c>
       <c r="E60">
+        <f t="shared" si="0"/>
+        <v>2468.049750000001</v>
+      </c>
+      <c r="F60">
         <f t="shared" si="1"/>
-        <v>2998.8650058333351</v>
-      </c>
-      <c r="F60">
-        <f t="shared" si="0"/>
-        <v>0.88201911936274557</v>
+        <v>0.72589698529411795</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -1714,12 +1714,12 @@
         <v>-3.3945500000000002</v>
       </c>
       <c r="E61">
+        <f t="shared" si="0"/>
+        <v>2458.6204444444456</v>
+      </c>
+      <c r="F61">
         <f t="shared" si="1"/>
-        <v>2998.3086768055573</v>
-      </c>
-      <c r="F61">
-        <f t="shared" si="0"/>
-        <v>0.88185549317810508</v>
+        <v>0.72312366013071927</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -1736,12 +1736,12 @@
         <v>-3.3948299999999998</v>
       </c>
       <c r="E62">
+        <f t="shared" si="0"/>
+        <v>2449.1903611111125</v>
+      </c>
+      <c r="F62">
         <f t="shared" si="1"/>
-        <v>2997.7428718055571</v>
-      </c>
-      <c r="F62">
-        <f t="shared" si="0"/>
-        <v>0.88168907994281087</v>
+        <v>0.72035010620915074</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -1758,12 +1758,12 @@
         <v>-3.3949099999999999</v>
       </c>
       <c r="E63">
+        <f t="shared" si="0"/>
+        <v>2439.7600555555568</v>
+      </c>
+      <c r="F63">
         <f t="shared" si="1"/>
-        <v>2997.1676231666684</v>
-      </c>
-      <c r="F63">
-        <f t="shared" si="0"/>
-        <v>0.88151988916666713</v>
+        <v>0.71757648692810494</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -1780,12 +1780,12 @@
         <v>-3.3948999999999998</v>
       </c>
       <c r="E64">
+        <f t="shared" si="0"/>
+        <v>2430.3297777777789</v>
+      </c>
+      <c r="F64">
         <f t="shared" si="1"/>
-        <v>2996.5829459444462</v>
-      </c>
-      <c r="F64">
-        <f t="shared" si="0"/>
-        <v>0.88134792527777828</v>
+        <v>0.71480287581699375</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
@@ -1802,12 +1802,12 @@
         <v>-3.39493</v>
       </c>
       <c r="E65">
+        <f t="shared" si="0"/>
+        <v>2420.8994166666675</v>
+      </c>
+      <c r="F65">
         <f t="shared" si="1"/>
-        <v>2995.9888331944462</v>
-      </c>
-      <c r="F65">
-        <f t="shared" si="0"/>
-        <v>0.8811731862336607</v>
+        <v>0.71202924019607872</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -1824,12 +1824,12 @@
         <v>-3.3949600000000002</v>
       </c>
       <c r="E66">
+        <f t="shared" si="0"/>
+        <v>2411.4689722222233</v>
+      </c>
+      <c r="F66">
         <f t="shared" si="1"/>
-        <v>2995.3852847500016</v>
-      </c>
-      <c r="F66">
-        <f t="shared" si="0"/>
-        <v>0.8809956719852946</v>
+        <v>0.70925558006535983</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -1846,12 +1846,12 @@
         <v>-3.39479</v>
       </c>
       <c r="E67">
-        <f t="shared" si="1"/>
-        <v>2994.7723365555571</v>
+        <f t="shared" si="0"/>
+        <v>2402.0390000000011</v>
       </c>
       <c r="F67">
         <f t="shared" ref="F67:F130" si="2">E67/3400</f>
-        <v>0.88081539310457557</v>
+        <v>0.70648205882352977</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
@@ -1868,12 +1868,12 @@
         <v>-3.3950100000000001</v>
       </c>
       <c r="E68">
-        <f t="shared" si="1"/>
-        <v>2994.149918055557</v>
+        <f t="shared" si="0"/>
+        <v>2392.6084166666678</v>
       </c>
       <c r="F68">
         <f t="shared" si="2"/>
-        <v>0.88063232883986975</v>
+        <v>0.70370835784313757</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
@@ -1890,12 +1890,12 @@
         <v>-3.3947699999999998</v>
       </c>
       <c r="E69">
-        <f t="shared" ref="E69:E132" si="3">E68+((A69/3600)*D69)</f>
-        <v>2993.5181136388906</v>
+        <f t="shared" ref="E69:E132" si="3">E68+((10/3600)*D69*1000)</f>
+        <v>2383.1785000000013</v>
       </c>
       <c r="F69">
         <f t="shared" si="2"/>
-        <v>0.88044650401143842</v>
+        <v>0.70093485294117686</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
@@ -1913,11 +1913,11 @@
       </c>
       <c r="E70">
         <f t="shared" si="3"/>
-        <v>2992.8768623055571</v>
+        <v>2373.7483333333348</v>
       </c>
       <c r="F70">
         <f t="shared" si="2"/>
-        <v>0.88025790067810505</v>
+        <v>0.69816127450980436</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
@@ -1935,11 +1935,11 @@
       </c>
       <c r="E71">
         <f t="shared" si="3"/>
-        <v>2992.2262076388906</v>
+        <v>2364.3185555555569</v>
       </c>
       <c r="F71">
         <f t="shared" si="2"/>
-        <v>0.88006653165849724</v>
+        <v>0.69538781045751674</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
@@ -1957,11 +1957,11 @@
       </c>
       <c r="E72">
         <f t="shared" si="3"/>
-        <v>2991.5660765277794</v>
+        <v>2354.8881111111127</v>
       </c>
       <c r="F72">
         <f t="shared" si="2"/>
-        <v>0.87987237544934693</v>
+        <v>0.69261415032679785</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
@@ -1979,11 +1979,11 @@
       </c>
       <c r="E73">
         <f t="shared" si="3"/>
-        <v>2990.8965090555571</v>
+        <v>2345.4575833333352</v>
       </c>
       <c r="F73">
         <f t="shared" si="2"/>
-        <v>0.87967544383986973</v>
+        <v>0.689840465686275</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -2001,11 +2001,11 @@
       </c>
       <c r="E74">
         <f t="shared" si="3"/>
-        <v>2990.2175690555573</v>
+        <v>2336.027861111113</v>
       </c>
       <c r="F74">
         <f t="shared" si="2"/>
-        <v>0.87947575560457569</v>
+        <v>0.68706701797385672</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -2023,11 +2023,11 @@
       </c>
       <c r="E75">
         <f t="shared" si="3"/>
-        <v>2989.529118222224</v>
+        <v>2326.5970277777797</v>
       </c>
       <c r="F75">
         <f t="shared" si="2"/>
-        <v>0.87927327006536005</v>
+        <v>0.68429324346405285</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
@@ -2045,11 +2045,11 @@
       </c>
       <c r="E76">
         <f t="shared" si="3"/>
-        <v>2988.8312673888909</v>
+        <v>2317.1666111111131</v>
       </c>
       <c r="F76">
         <f t="shared" si="2"/>
-        <v>0.87906801982026206</v>
+        <v>0.68151959150326857</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
@@ -2067,11 +2067,11 @@
       </c>
       <c r="E77">
         <f t="shared" si="3"/>
-        <v>2988.1240173888909</v>
+        <v>2307.7366111111132</v>
       </c>
       <c r="F77">
         <f t="shared" si="2"/>
-        <v>0.87886000511437967</v>
+        <v>0.6787460620915039</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
@@ -2089,11 +2089,11 @@
       </c>
       <c r="E78">
         <f t="shared" si="3"/>
-        <v>2987.40731627778</v>
+        <v>2298.3063333333353</v>
       </c>
       <c r="F78">
         <f t="shared" si="2"/>
-        <v>0.87864921066993529</v>
+        <v>0.67597245098039271</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
@@ -2111,11 +2111,11 @@
       </c>
       <c r="E79">
         <f t="shared" si="3"/>
-        <v>2986.6811870277797</v>
+        <v>2288.8760833333354</v>
       </c>
       <c r="F79">
         <f t="shared" si="2"/>
-        <v>0.87843564324346468</v>
+        <v>0.67319884803921626</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
@@ -2133,11 +2133,11 @@
       </c>
       <c r="E80">
         <f t="shared" si="3"/>
-        <v>2985.9456275277798</v>
+        <v>2279.4458333333355</v>
       </c>
       <c r="F80">
         <f t="shared" si="2"/>
-        <v>0.87821930221405287</v>
+        <v>0.6704252450980398</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
@@ -2155,11 +2155,11 @@
       </c>
       <c r="E81">
         <f t="shared" si="3"/>
-        <v>2985.2006663055577</v>
+        <v>2270.0159444444466</v>
       </c>
       <c r="F81">
         <f t="shared" si="2"/>
-        <v>0.8780001959722229</v>
+        <v>0.66765174836601371</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
@@ -2177,11 +2177,11 @@
       </c>
       <c r="E82">
         <f t="shared" si="3"/>
-        <v>2984.4462418611133</v>
+        <v>2260.585638888891</v>
       </c>
       <c r="F82">
         <f t="shared" si="2"/>
-        <v>0.8777783064297392</v>
+        <v>0.66487812908496791</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
@@ -2199,11 +2199,11 @@
       </c>
       <c r="E83">
         <f t="shared" si="3"/>
-        <v>2983.6824051111134</v>
+        <v>2251.1555555555578</v>
       </c>
       <c r="F83">
         <f t="shared" si="2"/>
-        <v>0.87755364856209217</v>
+        <v>0.66210457516339938</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
@@ -2221,11 +2221,11 @@
       </c>
       <c r="E84">
         <f t="shared" si="3"/>
-        <v>2982.909090444447</v>
+        <v>2241.7248888888912</v>
       </c>
       <c r="F84">
         <f t="shared" si="2"/>
-        <v>0.87732620307189613</v>
+        <v>0.65933084967320332</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
@@ -2243,11 +2243,11 @@
       </c>
       <c r="E85">
         <f t="shared" si="3"/>
-        <v>2982.1264027500024</v>
+        <v>2232.294916666669</v>
       </c>
       <c r="F85">
         <f t="shared" si="2"/>
-        <v>0.87709600080882422</v>
+        <v>0.65655732843137327</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
@@ -2265,11 +2265,11 @@
       </c>
       <c r="E86">
         <f t="shared" si="3"/>
-        <v>2981.3342757500022</v>
+        <v>2222.8648333333358</v>
       </c>
       <c r="F86">
         <f t="shared" si="2"/>
-        <v>0.87686302227941237</v>
+        <v>0.65378377450980463</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
@@ -2287,11 +2287,11 @@
       </c>
       <c r="E87">
         <f t="shared" si="3"/>
-        <v>2980.5327139444466</v>
+        <v>2213.4346944444469</v>
       </c>
       <c r="F87">
         <f t="shared" si="2"/>
-        <v>0.87662726880719022</v>
+        <v>0.65101020424836675</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
@@ -2309,11 +2309,11 @@
       </c>
       <c r="E88">
         <f t="shared" si="3"/>
-        <v>2979.7217100555577</v>
+        <v>2204.0044166666689</v>
       </c>
       <c r="F88">
         <f t="shared" si="2"/>
-        <v>0.87638873825163466</v>
+        <v>0.64823659313725557</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
@@ -2331,11 +2331,11 @@
       </c>
       <c r="E89">
         <f t="shared" si="3"/>
-        <v>2978.9013024722244</v>
+        <v>2194.5744444444467</v>
       </c>
       <c r="F89">
         <f t="shared" si="2"/>
-        <v>0.87614744190359539</v>
+        <v>0.64546307189542551</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
@@ -2353,11 +2353,11 @@
       </c>
       <c r="E90">
         <f t="shared" si="3"/>
-        <v>2978.0714258055577</v>
+        <v>2185.1440277777801</v>
       </c>
       <c r="F90">
         <f t="shared" si="2"/>
-        <v>0.87590336053104645</v>
+        <v>0.64268941993464124</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
@@ -2375,11 +2375,11 @@
       </c>
       <c r="E91">
         <f t="shared" si="3"/>
-        <v>2977.2321187222242</v>
+        <v>2175.7136111111136</v>
       </c>
       <c r="F91">
         <f t="shared" si="2"/>
-        <v>0.87565650550653651</v>
+        <v>0.63991576797385696</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
@@ -2397,11 +2397,11 @@
       </c>
       <c r="E92">
         <f t="shared" si="3"/>
-        <v>2976.3834162222242</v>
+        <v>2166.2835833333356</v>
       </c>
       <c r="F92">
         <f t="shared" si="2"/>
-        <v>0.87540688712418357</v>
+        <v>0.63714223039215756</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
@@ -2419,11 +2419,11 @@
       </c>
       <c r="E93">
         <f t="shared" si="3"/>
-        <v>2975.5252735833355</v>
+        <v>2156.8534444444467</v>
       </c>
       <c r="F93">
         <f t="shared" si="2"/>
-        <v>0.87515449223039277</v>
+        <v>0.63436866013071957</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
@@ -2441,11 +2441,11 @@
       </c>
       <c r="E94">
         <f t="shared" si="3"/>
-        <v>2974.6576701388913</v>
+        <v>2147.4229722222244</v>
       </c>
       <c r="F94">
         <f t="shared" si="2"/>
-        <v>0.87489931474673277</v>
+        <v>0.63159499183006595</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="E95">
         <f t="shared" si="3"/>
-        <v>2973.7807059722245</v>
+        <v>2137.9932500000023</v>
       </c>
       <c r="F95">
         <f t="shared" si="2"/>
-        <v>0.87464138410947778</v>
+        <v>0.62882154411764768</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
@@ -2485,11 +2485,11 @@
       </c>
       <c r="E96">
         <f t="shared" si="3"/>
-        <v>2972.8942859722247</v>
+        <v>2128.5632500000024</v>
       </c>
       <c r="F96">
         <f t="shared" si="2"/>
-        <v>0.87438067234477201</v>
+        <v>0.62604801470588312</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
@@ -2507,11 +2507,11 @@
       </c>
       <c r="E97">
         <f t="shared" si="3"/>
-        <v>2971.9984570833358</v>
+        <v>2119.1334722222246</v>
       </c>
       <c r="F97">
         <f t="shared" si="2"/>
-        <v>0.87411719325980464</v>
+        <v>0.62327455065359549</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
@@ -2529,11 +2529,11 @@
       </c>
       <c r="E98">
         <f t="shared" si="3"/>
-        <v>2971.0931744166692</v>
+        <v>2109.7034444444466</v>
       </c>
       <c r="F98">
         <f t="shared" si="2"/>
-        <v>0.87385093365196154</v>
+        <v>0.62050101307189609</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
@@ -2551,11 +2551,11 @@
       </c>
       <c r="E99">
         <f t="shared" si="3"/>
-        <v>2970.1785048333359</v>
+        <v>2100.2738611111131</v>
       </c>
       <c r="F99">
         <f t="shared" si="2"/>
-        <v>0.87358191318627521</v>
+        <v>0.6177276062091509</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
@@ -2573,11 +2573,11 @@
       </c>
       <c r="E100">
         <f t="shared" si="3"/>
-        <v>2969.2543539444468</v>
+        <v>2090.8437500000018</v>
       </c>
       <c r="F100">
         <f t="shared" si="2"/>
-        <v>0.87331010410130794</v>
+        <v>0.61495404411764765</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
@@ -2595,11 +2595,11 @@
       </c>
       <c r="E101">
         <f t="shared" si="3"/>
-        <v>2968.3207426944468</v>
+        <v>2081.4133333333352</v>
       </c>
       <c r="F101">
         <f t="shared" si="2"/>
-        <v>0.87303551255719025</v>
+        <v>0.61218039215686326</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
@@ -2617,11 +2617,11 @@
       </c>
       <c r="E102">
         <f t="shared" si="3"/>
-        <v>2967.3776899166692</v>
+        <v>2071.9828055555577</v>
       </c>
       <c r="F102">
         <f t="shared" si="2"/>
-        <v>0.87275814409313801</v>
+        <v>0.60940670751634052</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
@@ -2639,11 +2639,11 @@
       </c>
       <c r="E103">
         <f t="shared" si="3"/>
-        <v>2966.4252122222247</v>
+        <v>2062.5523333333354</v>
       </c>
       <c r="F103">
         <f t="shared" si="2"/>
-        <v>0.87247800359477201</v>
+        <v>0.6066330392156869</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
@@ -2661,11 +2661,11 @@
       </c>
       <c r="E104">
         <f t="shared" si="3"/>
-        <v>2965.4633862222245</v>
+        <v>2053.1226666666685</v>
       </c>
       <c r="F104">
         <f t="shared" si="2"/>
-        <v>0.87219511359477186</v>
+        <v>0.60385960784313775</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
@@ -2683,11 +2683,11 @@
       </c>
       <c r="E105">
         <f t="shared" si="3"/>
-        <v>2964.4920990833357</v>
+        <v>2043.6926944444463</v>
       </c>
       <c r="F105">
         <f t="shared" si="2"/>
-        <v>0.8719094409068634</v>
+        <v>0.60108608660130769</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
@@ -2705,11 +2705,11 @@
       </c>
       <c r="E106">
         <f t="shared" si="3"/>
-        <v>2963.5113819722246</v>
+        <v>2034.2627222222241</v>
       </c>
       <c r="F106">
         <f t="shared" si="2"/>
-        <v>0.87162099469771315</v>
+        <v>0.59831256535947763</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
@@ -2727,11 +2727,11 @@
       </c>
       <c r="E107">
         <f t="shared" si="3"/>
-        <v>2962.5212465555578</v>
+        <v>2024.8328611111128</v>
       </c>
       <c r="F107">
         <f t="shared" si="2"/>
-        <v>0.87132977839869352</v>
+        <v>0.59553907679738616</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
@@ -2749,11 +2749,11 @@
       </c>
       <c r="E108">
         <f t="shared" si="3"/>
-        <v>2961.5216282777801</v>
+        <v>2015.4025000000017</v>
       </c>
       <c r="F108">
         <f t="shared" si="2"/>
-        <v>0.87103577302287649</v>
+        <v>0.59276544117647112</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
@@ -2771,11 +2771,11 @@
       </c>
       <c r="E109">
         <f t="shared" si="3"/>
-        <v>2960.5126004444469</v>
+        <v>2005.972333333335</v>
       </c>
       <c r="F109">
         <f t="shared" si="2"/>
-        <v>0.8707390001307197</v>
+        <v>0.58999186274509852</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
@@ -2793,11 +2793,11 @@
       </c>
       <c r="E110">
         <f t="shared" si="3"/>
-        <v>2959.4941544444468</v>
+        <v>1996.5422777777794</v>
       </c>
       <c r="F110">
         <f t="shared" si="2"/>
-        <v>0.87043945718954319</v>
+        <v>0.5872183169934645</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
@@ -2815,11 +2815,11 @@
       </c>
       <c r="E111">
         <f t="shared" si="3"/>
-        <v>2958.4662148055581</v>
+        <v>1987.1116388888906</v>
       </c>
       <c r="F111">
         <f t="shared" si="2"/>
-        <v>0.87013712200163473</v>
+        <v>0.58444459967320317</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
@@ -2837,11 +2837,11 @@
       </c>
       <c r="E112">
         <f t="shared" si="3"/>
-        <v>2957.4288934166693</v>
+        <v>1977.6814444444462</v>
       </c>
       <c r="F112">
         <f t="shared" si="2"/>
-        <v>0.86983202747549093</v>
+        <v>0.58167101307189595</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
@@ -2859,11 +2859,11 @@
       </c>
       <c r="E113">
         <f t="shared" si="3"/>
-        <v>2956.3821171666691</v>
+        <v>1968.2510277777797</v>
       </c>
       <c r="F113">
         <f t="shared" si="2"/>
-        <v>0.86952415210784384</v>
+        <v>0.57889736111111167</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
@@ -2881,11 +2881,11 @@
       </c>
       <c r="E114">
         <f t="shared" si="3"/>
-        <v>2955.3259011666692</v>
+        <v>1958.8205277777797</v>
       </c>
       <c r="F114">
         <f t="shared" si="2"/>
-        <v>0.86921350034313793</v>
+        <v>0.57612368464052344</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
@@ -2903,11 +2903,11 @@
       </c>
       <c r="E115">
         <f t="shared" si="3"/>
-        <v>2954.2603174444471</v>
+        <v>1949.3905833333354</v>
       </c>
       <c r="F115">
         <f t="shared" si="2"/>
-        <v>0.86890009336601381</v>
+        <v>0.573350171568628</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
@@ -2925,11 +2925,11 @@
       </c>
       <c r="E116">
         <f t="shared" si="3"/>
-        <v>2953.1852847777805</v>
+        <v>1939.9604722222243</v>
       </c>
       <c r="F116">
         <f t="shared" si="2"/>
-        <v>0.8685839072875825</v>
+        <v>0.57057660947712485</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
@@ -2947,11 +2947,11 @@
       </c>
       <c r="E117">
         <f t="shared" si="3"/>
-        <v>2952.1008251944472</v>
+        <v>1930.5303888888909</v>
       </c>
       <c r="F117">
         <f t="shared" si="2"/>
-        <v>0.86826494858660208</v>
+        <v>0.5678030555555561</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
@@ -2969,11 +2969,11 @@
       </c>
       <c r="E118">
         <f t="shared" si="3"/>
-        <v>2951.0069548611141</v>
+        <v>1921.1004722222242</v>
       </c>
       <c r="F118">
         <f t="shared" si="2"/>
-        <v>0.86794322201797469</v>
+        <v>0.56502955065359539</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
@@ -2991,11 +2991,11 @@
       </c>
       <c r="E119">
         <f t="shared" si="3"/>
-        <v>2949.9036611111142</v>
+        <v>1911.670611111113</v>
       </c>
       <c r="F119">
         <f t="shared" si="2"/>
-        <v>0.86761872385621008</v>
+        <v>0.56225606209150381</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
@@ -3013,11 +3013,11 @@
       </c>
       <c r="E120">
         <f t="shared" si="3"/>
-        <v>2948.7908785000031</v>
+        <v>1902.2402500000019</v>
       </c>
       <c r="F120">
         <f t="shared" si="2"/>
-        <v>0.86729143485294213</v>
+        <v>0.55948242647058877</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
@@ -3035,11 +3035,11 @@
       </c>
       <c r="E121">
         <f t="shared" si="3"/>
-        <v>2947.6686721388919</v>
+        <v>1892.8099444444463</v>
       </c>
       <c r="F121">
         <f t="shared" si="2"/>
-        <v>0.86696137415849761</v>
+        <v>0.55670880718954308</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
@@ -3057,11 +3057,11 @@
       </c>
       <c r="E122">
         <f t="shared" si="3"/>
-        <v>2946.5370688055586</v>
+        <v>1883.3799166666686</v>
       </c>
       <c r="F122">
         <f t="shared" si="2"/>
-        <v>0.86662854964869374</v>
+        <v>0.55393526960784367</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
@@ -3079,11 +3079,11 @@
       </c>
       <c r="E123">
         <f t="shared" si="3"/>
-        <v>2945.3960589722251</v>
+        <v>1873.9500833333352</v>
       </c>
       <c r="F123">
         <f t="shared" si="2"/>
-        <v>0.86629295852124266</v>
+        <v>0.55116178921568681</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
@@ -3101,11 +3101,11 @@
       </c>
       <c r="E124">
         <f t="shared" si="3"/>
-        <v>2944.2456193055586</v>
+        <v>1864.5202500000019</v>
       </c>
       <c r="F124">
         <f t="shared" si="2"/>
-        <v>0.86595459391339957</v>
+        <v>0.54838830882352996</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
@@ -3123,11 +3123,11 @@
       </c>
       <c r="E125">
         <f t="shared" si="3"/>
-        <v>2943.0857224722254</v>
+        <v>1855.0901944444463</v>
       </c>
       <c r="F125">
         <f t="shared" si="2"/>
-        <v>0.86561344778594862</v>
+        <v>0.54561476307189594</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
@@ -3145,11 +3145,11 @@
       </c>
       <c r="E126">
         <f t="shared" si="3"/>
-        <v>2941.9164093611143</v>
+        <v>1845.660250000002</v>
       </c>
       <c r="F126">
         <f t="shared" si="2"/>
-        <v>0.86526953216503366</v>
+        <v>0.54284125000000061</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
@@ -3167,11 +3167,11 @@
       </c>
       <c r="E127">
         <f t="shared" si="3"/>
-        <v>2940.7376385277812</v>
+        <v>1836.2300833333352</v>
       </c>
       <c r="F127">
         <f t="shared" si="2"/>
-        <v>0.8649228348611121</v>
+        <v>0.540067671568628</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.35">
@@ -3189,11 +3189,11 @@
       </c>
       <c r="E128">
         <f t="shared" si="3"/>
-        <v>2939.5494935277811</v>
+        <v>1826.800361111113</v>
       </c>
       <c r="F128">
         <f t="shared" si="2"/>
-        <v>0.8645733804493474</v>
+        <v>0.53729422385620973</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.35">
@@ -3211,11 +3211,11 @@
       </c>
       <c r="E129">
         <f t="shared" si="3"/>
-        <v>2938.3518729444477</v>
+        <v>1817.3702777777796</v>
       </c>
       <c r="F129">
         <f t="shared" si="2"/>
-        <v>0.86422113910130816</v>
+        <v>0.53452066993464109</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.35">
@@ -3233,11 +3233,11 @@
       </c>
       <c r="E130">
         <f t="shared" si="3"/>
-        <v>2937.144861388892</v>
+        <v>1807.9405000000017</v>
       </c>
       <c r="F130">
         <f t="shared" si="2"/>
-        <v>0.86386613570261528</v>
+        <v>0.53174720588235347</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
@@ -3255,11 +3255,11 @@
       </c>
       <c r="E131">
         <f t="shared" si="3"/>
-        <v>2935.9284021388921</v>
+        <v>1798.510583333335</v>
       </c>
       <c r="F131">
         <f t="shared" ref="F131:F194" si="4">E131/3400</f>
-        <v>0.86350835357026234</v>
+        <v>0.52897370098039265</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.35">
@@ -3277,11 +3277,11 @@
       </c>
       <c r="E132">
         <f t="shared" si="3"/>
-        <v>2934.7025454722257</v>
+        <v>1789.0809166666684</v>
       </c>
       <c r="F132">
         <f t="shared" si="4"/>
-        <v>0.86314780749183107</v>
+        <v>0.52620026960784361</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.35">
@@ -3298,12 +3298,12 @@
         <v>-3.3948499999999999</v>
       </c>
       <c r="E133">
-        <f t="shared" ref="E133:E196" si="5">E132+((A133/3600)*D133)</f>
-        <v>2933.467197277781</v>
+        <f t="shared" ref="E133:E196" si="5">E132+((10/3600)*D133*1000)</f>
+        <v>1779.6507777777795</v>
       </c>
       <c r="F133">
         <f t="shared" si="4"/>
-        <v>0.86278446978758261</v>
+        <v>0.52342669934640573</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.35">
@@ -3321,11 +3321,11 @@
       </c>
       <c r="E134">
         <f t="shared" si="5"/>
-        <v>2932.2224666111142</v>
+        <v>1770.2210000000016</v>
       </c>
       <c r="F134">
         <f t="shared" si="4"/>
-        <v>0.86241837253268061</v>
+        <v>0.52065323529411811</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.35">
@@ -3343,11 +3343,11 @@
       </c>
       <c r="E135">
         <f t="shared" si="5"/>
-        <v>2930.9682138055587</v>
+        <v>1760.7905277777793</v>
       </c>
       <c r="F135">
         <f t="shared" si="4"/>
-        <v>0.86204947464869375</v>
+        <v>0.51787956699346449</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
@@ -3365,11 +3365,11 @@
       </c>
       <c r="E136">
         <f t="shared" si="5"/>
-        <v>2929.7045789166696</v>
+        <v>1751.3604166666682</v>
       </c>
       <c r="F136">
         <f t="shared" si="4"/>
-        <v>0.86167781732843218</v>
+        <v>0.51510600490196123</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
@@ -3387,11 +3387,11 @@
       </c>
       <c r="E137">
         <f t="shared" si="5"/>
-        <v>2928.4315101666693</v>
+        <v>1741.9302777777793</v>
       </c>
       <c r="F137">
         <f t="shared" si="4"/>
-        <v>0.86130338534313799</v>
+        <v>0.51233243464052336</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
@@ -3409,11 +3409,11 @@
       </c>
       <c r="E138">
         <f t="shared" si="5"/>
-        <v>2927.1489319444472</v>
+        <v>1732.4995555555572</v>
       </c>
       <c r="F138">
         <f t="shared" si="4"/>
-        <v>0.86092615645424919</v>
+        <v>0.50955869281045796</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
@@ -3431,11 +3431,11 @@
       </c>
       <c r="E139">
         <f t="shared" si="5"/>
-        <v>2925.8571170833361</v>
+        <v>1723.0702500000016</v>
       </c>
       <c r="F139">
         <f t="shared" si="4"/>
-        <v>0.86054621090686356</v>
+        <v>0.50678536764705928</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.35">
@@ -3453,11 +3453,11 @@
       </c>
       <c r="E140">
         <f t="shared" si="5"/>
-        <v>2924.5557732500029</v>
+        <v>1713.6402222222239</v>
       </c>
       <c r="F140">
         <f t="shared" si="4"/>
-        <v>0.86016346272058908</v>
+        <v>0.50401183006535999</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.35">
@@ -3475,11 +3475,11 @@
       </c>
       <c r="E141">
         <f t="shared" si="5"/>
-        <v>2923.245014833336</v>
+        <v>1704.2103055555572</v>
       </c>
       <c r="F141">
         <f t="shared" si="4"/>
-        <v>0.85977794553921649</v>
+        <v>0.50123832516339917</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.35">
@@ -3497,11 +3497,11 @@
       </c>
       <c r="E142">
         <f t="shared" si="5"/>
-        <v>2921.9248731666694</v>
+        <v>1694.7807222222239</v>
       </c>
       <c r="F142">
         <f t="shared" si="4"/>
-        <v>0.85938966857843213</v>
+        <v>0.49846491830065409</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.35">
@@ -3519,11 +3519,11 @@
       </c>
       <c r="E143">
         <f t="shared" si="5"/>
-        <v>2920.595188333336</v>
+        <v>1685.3503333333349</v>
       </c>
       <c r="F143">
         <f t="shared" si="4"/>
-        <v>0.85899858480392233</v>
+        <v>0.49569127450980438</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.35">
@@ -3541,11 +3541,11 @@
       </c>
       <c r="E144">
         <f t="shared" si="5"/>
-        <v>2919.2561401666694</v>
+        <v>1675.9204166666682</v>
       </c>
       <c r="F144">
         <f t="shared" si="4"/>
-        <v>0.85860474710784396</v>
+        <v>0.49291776960784356</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.35">
@@ -3563,11 +3563,11 @@
       </c>
       <c r="E145">
         <f t="shared" si="5"/>
-        <v>2917.9076303055581</v>
+        <v>1666.4902777777793</v>
       </c>
       <c r="F145">
         <f t="shared" si="4"/>
-        <v>0.85820812656045831</v>
+        <v>0.49014419934640568</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.35">
@@ -3585,11 +3585,11 @@
       </c>
       <c r="E146">
         <f t="shared" si="5"/>
-        <v>2916.5497063055582</v>
+        <v>1657.0602500000016</v>
       </c>
       <c r="F146">
         <f t="shared" si="4"/>
-        <v>0.85780873714869355</v>
+        <v>0.48737066176470634</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.35">
@@ -3607,11 +3607,11 @@
       </c>
       <c r="E147">
         <f t="shared" si="5"/>
-        <v>2915.1822717222249</v>
+        <v>1647.6296666666683</v>
       </c>
       <c r="F147">
         <f t="shared" si="4"/>
-        <v>0.85740655050653669</v>
+        <v>0.48459696078431419</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.35">
@@ -3629,11 +3629,11 @@
       </c>
       <c r="E148">
         <f t="shared" si="5"/>
-        <v>2913.8054065555584</v>
+        <v>1638.199083333335</v>
       </c>
       <c r="F148">
         <f t="shared" si="4"/>
-        <v>0.8570015901633995</v>
+        <v>0.48182325980392204</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.35">
@@ -3651,11 +3651,11 @@
       </c>
       <c r="E149">
         <f t="shared" si="5"/>
-        <v>2912.4192006388917</v>
+        <v>1628.7691111111128</v>
       </c>
       <c r="F149">
         <f t="shared" si="4"/>
-        <v>0.85659388254085045</v>
+        <v>0.47904973856209199</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.35">
@@ -3673,11 +3673,11 @@
       </c>
       <c r="E150">
         <f t="shared" si="5"/>
-        <v>2911.0235935277806</v>
+        <v>1619.3393333333349</v>
       </c>
       <c r="F150">
         <f t="shared" si="4"/>
-        <v>0.85618340986111197</v>
+        <v>0.47627627450980436</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.35">
@@ -3695,11 +3695,11 @@
       </c>
       <c r="E151">
         <f t="shared" si="5"/>
-        <v>2909.6184490277806</v>
+        <v>1609.908833333335</v>
       </c>
       <c r="F151">
         <f t="shared" si="4"/>
-        <v>0.85577013206699426</v>
+        <v>0.47350259803921618</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.35">
@@ -3717,11 +3717,11 @@
       </c>
       <c r="E152">
         <f t="shared" si="5"/>
-        <v>2908.2039156944475</v>
+        <v>1600.4786111111127</v>
       </c>
       <c r="F152">
         <f t="shared" si="4"/>
-        <v>0.85535409285130803</v>
+        <v>0.47072900326797434</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.35">
@@ -3739,11 +3739,11 @@
       </c>
       <c r="E153">
         <f t="shared" si="5"/>
-        <v>2906.7800024722251</v>
+        <v>1591.0487222222239</v>
       </c>
       <c r="F153">
         <f t="shared" si="4"/>
-        <v>0.85493529484477204</v>
+        <v>0.4679555065359482</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.35">
@@ -3761,11 +3761,11 @@
       </c>
       <c r="E154">
         <f t="shared" si="5"/>
-        <v>2905.3466466944474</v>
+        <v>1581.6187500000017</v>
       </c>
       <c r="F154">
         <f t="shared" si="4"/>
-        <v>0.85451371961601397</v>
+        <v>0.46518198529411814</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.35">
@@ -3783,11 +3783,11 @@
       </c>
       <c r="E155">
         <f t="shared" si="5"/>
-        <v>2903.9038226944472</v>
+        <v>1572.1885277777794</v>
       </c>
       <c r="F155">
         <f t="shared" si="4"/>
-        <v>0.85408935961601384</v>
+        <v>0.4624083905228763</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.35">
@@ -3805,11 +3805,11 @@
       </c>
       <c r="E156">
         <f t="shared" si="5"/>
-        <v>2902.4515984166692</v>
+        <v>1562.7585000000017</v>
       </c>
       <c r="F156">
         <f t="shared" si="4"/>
-        <v>0.85366223482843206</v>
+        <v>0.45963485294117695</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.35">
@@ -3827,11 +3827,11 @@
       </c>
       <c r="E157">
         <f t="shared" si="5"/>
-        <v>2900.9899613333359</v>
+        <v>1553.328583333335</v>
       </c>
       <c r="F157">
         <f t="shared" si="4"/>
-        <v>0.85323234156862826</v>
+        <v>0.45686134803921619</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.35">
@@ -3849,11 +3849,11 @@
       </c>
       <c r="E158">
         <f t="shared" si="5"/>
-        <v>2899.5188640000024</v>
+        <v>1543.898472222224</v>
       </c>
       <c r="F158">
         <f t="shared" si="4"/>
-        <v>0.85279966588235367</v>
+        <v>0.45408778594771293</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.35">
@@ -3871,11 +3871,11 @@
       </c>
       <c r="E159">
         <f t="shared" si="5"/>
-        <v>2898.0383321944469</v>
+        <v>1534.4683333333351</v>
       </c>
       <c r="F159">
         <f t="shared" si="4"/>
-        <v>0.85236421535130791</v>
+        <v>0.451314215686275</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.35">
@@ -3893,11 +3893,11 @@
       </c>
       <c r="E160">
         <f t="shared" si="5"/>
-        <v>2896.5483483055582</v>
+        <v>1525.0380555555573</v>
       </c>
       <c r="F160">
         <f t="shared" si="4"/>
-        <v>0.85192598479575243</v>
+        <v>0.44854060457516393</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.35">
@@ -3915,11 +3915,11 @@
       </c>
       <c r="E161">
         <f t="shared" si="5"/>
-        <v>2895.0489738888914</v>
+        <v>1515.6080277777796</v>
       </c>
       <c r="F161">
         <f t="shared" si="4"/>
-        <v>0.8514849923202622</v>
+        <v>0.44576706699346458</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.35">
@@ -3937,11 +3937,11 @@
       </c>
       <c r="E162">
         <f t="shared" si="5"/>
-        <v>2893.5401738888913</v>
+        <v>1506.1780277777796</v>
       </c>
       <c r="F162">
         <f t="shared" si="4"/>
-        <v>0.85104122761437984</v>
+        <v>0.44299353758169985</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.35">
@@ -3959,11 +3959,11 @@
       </c>
       <c r="E163">
         <f t="shared" si="5"/>
-        <v>2892.0220243888912</v>
+        <v>1496.7485277777796</v>
       </c>
       <c r="F163">
         <f t="shared" si="4"/>
-        <v>0.85059471305555623</v>
+        <v>0.44022015522875868</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.35">
@@ -3981,11 +3981,11 @@
       </c>
       <c r="E164">
         <f t="shared" si="5"/>
-        <v>2890.4943733888913</v>
+        <v>1487.3185833333353</v>
       </c>
       <c r="F164">
         <f t="shared" si="4"/>
-        <v>0.85014540393790916</v>
+        <v>0.4374466421568633</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.35">
@@ -4003,11 +4003,11 @@
       </c>
       <c r="E165">
         <f t="shared" si="5"/>
-        <v>2888.9572833888915</v>
+        <v>1477.8885833333352</v>
       </c>
       <c r="F165">
         <f t="shared" si="4"/>
-        <v>0.84969331864379161</v>
+        <v>0.43467311274509857</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.35">
@@ -4025,11 +4025,11 @@
       </c>
       <c r="E166">
         <f t="shared" si="5"/>
-        <v>2887.4107269444471</v>
+        <v>1468.4583611111129</v>
       </c>
       <c r="F166">
         <f t="shared" si="4"/>
-        <v>0.84923844910130797</v>
+        <v>0.43189951797385673</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.35">
@@ -4047,11 +4047,11 @@
       </c>
       <c r="E167">
         <f t="shared" si="5"/>
-        <v>2885.8546806944473</v>
+        <v>1459.0277777777796</v>
       </c>
       <c r="F167">
         <f t="shared" si="4"/>
-        <v>0.8487807884395433</v>
+        <v>0.42912581699346458</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.35">
@@ -4069,11 +4069,11 @@
       </c>
       <c r="E168">
         <f t="shared" si="5"/>
-        <v>2884.2892776388917</v>
+        <v>1449.5976388888907</v>
       </c>
       <c r="F168">
         <f t="shared" si="4"/>
-        <v>0.84832037577614461</v>
+        <v>0.42635224673202671</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.35">
@@ -4091,11 +4091,11 @@
       </c>
       <c r="E169">
         <f t="shared" si="5"/>
-        <v>2882.7145604166694</v>
+        <v>1440.1681944444463</v>
       </c>
       <c r="F169">
         <f t="shared" si="4"/>
-        <v>0.84785722365196159</v>
+        <v>0.42357888071895478</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.35">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="E170">
         <f t="shared" si="5"/>
-        <v>2881.130409083336</v>
+        <v>1430.7387222222239</v>
       </c>
       <c r="F170">
         <f t="shared" si="4"/>
-        <v>0.84739129678921643</v>
+        <v>0.42080550653594823</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.35">
@@ -4135,11 +4135,11 @@
       </c>
       <c r="E171">
         <f t="shared" si="5"/>
-        <v>2879.536696833336</v>
+        <v>1421.3084722222238</v>
       </c>
       <c r="F171">
         <f t="shared" si="4"/>
-        <v>0.84692255789215765</v>
+        <v>0.41803190359477171</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.35">
@@ -4157,11 +4157,11 @@
       </c>
       <c r="E172">
         <f t="shared" si="5"/>
-        <v>2877.9335401666694</v>
+        <v>1411.8781388888906</v>
       </c>
       <c r="F172">
         <f t="shared" si="4"/>
-        <v>0.84645104122549097</v>
+        <v>0.41525827614379135</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.35">
@@ -4179,11 +4179,11 @@
       </c>
       <c r="E173">
         <f t="shared" si="5"/>
-        <v>2876.3210481666692</v>
+        <v>1402.4483611111127</v>
       </c>
       <c r="F173">
         <f t="shared" si="4"/>
-        <v>0.84597677887254974</v>
+        <v>0.41248481209150373</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.35">
@@ -4201,11 +4201,11 @@
       </c>
       <c r="E174">
         <f t="shared" si="5"/>
-        <v>2874.6990881666693</v>
+        <v>1393.0183611111127</v>
       </c>
       <c r="F174">
         <f t="shared" si="4"/>
-        <v>0.84549973181372629</v>
+        <v>0.409711282679739</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.35">
@@ -4223,11 +4223,11 @@
       </c>
       <c r="E175">
         <f t="shared" si="5"/>
-        <v>2873.0676501111138</v>
+        <v>1383.5880833333349</v>
       </c>
       <c r="F175">
         <f t="shared" si="4"/>
-        <v>0.84501989709150405</v>
+        <v>0.40693767156862792</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.35">
@@ -4245,11 +4245,11 @@
       </c>
       <c r="E176">
         <f t="shared" si="5"/>
-        <v>2871.4268542777804</v>
+        <v>1374.1582222222237</v>
       </c>
       <c r="F176">
         <f t="shared" si="4"/>
-        <v>0.84453731008170008</v>
+        <v>0.40416418300653639</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.35">
@@ -4267,11 +4267,11 @@
       </c>
       <c r="E177">
         <f t="shared" si="5"/>
-        <v>2869.7767015000027</v>
+        <v>1364.7287777777792</v>
       </c>
       <c r="F177">
         <f t="shared" si="4"/>
-        <v>0.84405197102941254</v>
+        <v>0.40139081699346446</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.35">
@@ -4289,11 +4289,11 @@
       </c>
       <c r="E178">
         <f t="shared" si="5"/>
-        <v>2868.1170606111136</v>
+        <v>1355.2990000000013</v>
       </c>
       <c r="F178">
         <f t="shared" si="4"/>
-        <v>0.84356384135620988</v>
+        <v>0.39861735294117684</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.35">
@@ -4311,11 +4311,11 @@
       </c>
       <c r="E179">
         <f t="shared" si="5"/>
-        <v>2866.4479555277803</v>
+        <v>1345.8690277777791</v>
       </c>
       <c r="F179">
         <f t="shared" si="4"/>
-        <v>0.84307292809640599</v>
+        <v>0.39584383169934678</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.35">
@@ -4333,11 +4333,11 @@
       </c>
       <c r="E180">
         <f t="shared" si="5"/>
-        <v>2864.7692078611135</v>
+        <v>1336.4378611111124</v>
       </c>
       <c r="F180">
         <f t="shared" si="4"/>
-        <v>0.8425791787826804</v>
+        <v>0.39306995915032716</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.35">
@@ -4355,11 +4355,11 @@
       </c>
       <c r="E181">
         <f t="shared" si="5"/>
-        <v>2863.0811732222246</v>
+        <v>1327.0075000000013</v>
       </c>
       <c r="F181">
         <f t="shared" si="4"/>
-        <v>0.84208269800653668</v>
+        <v>0.39029632352941213</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.35">
@@ -4377,11 +4377,11 @@
       </c>
       <c r="E182">
         <f t="shared" si="5"/>
-        <v>2861.3837382222246</v>
+        <v>1317.5773055555569</v>
       </c>
       <c r="F182">
         <f t="shared" si="4"/>
-        <v>0.84158345241830135</v>
+        <v>0.38752273692810496</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.35">
@@ -4399,11 +4399,11 @@
       </c>
       <c r="E183">
         <f t="shared" si="5"/>
-        <v>2859.6767925833356</v>
+        <v>1308.1466666666681</v>
       </c>
       <c r="F183">
         <f t="shared" si="4"/>
-        <v>0.84108140958333399</v>
+        <v>0.38474901960784358</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.35">
@@ -4421,11 +4421,11 @@
       </c>
       <c r="E184">
         <f t="shared" si="5"/>
-        <v>2857.9604971944468</v>
+        <v>1298.7164722222237</v>
       </c>
       <c r="F184">
         <f t="shared" si="4"/>
-        <v>0.84057661682189611</v>
+        <v>0.38197543300653641</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.35">
@@ -4443,11 +4443,11 @@
       </c>
       <c r="E185">
         <f t="shared" si="5"/>
-        <v>2856.2346902777804</v>
+        <v>1289.2858333333349</v>
       </c>
       <c r="F185">
         <f t="shared" si="4"/>
-        <v>0.84006902655228832</v>
+        <v>0.37920171568627498</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.35">
@@ -4465,11 +4465,11 @@
       </c>
       <c r="E186">
         <f t="shared" si="5"/>
-        <v>2854.4996520555583</v>
+        <v>1279.8562777777795</v>
       </c>
       <c r="F186">
         <f t="shared" si="4"/>
-        <v>0.83955872119281127</v>
+        <v>0.37642831699346457</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.35">
@@ -4487,11 +4487,11 @@
       </c>
       <c r="E187">
         <f t="shared" si="5"/>
-        <v>2852.755112333336</v>
+        <v>1270.4263333333352</v>
       </c>
       <c r="F187">
         <f t="shared" si="4"/>
-        <v>0.83904562127451054</v>
+        <v>0.37365480392156919</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.35">
@@ -4509,11 +4509,11 @@
       </c>
       <c r="E188">
         <f t="shared" si="5"/>
-        <v>2851.0011426666692</v>
+        <v>1260.9963888888908</v>
       </c>
       <c r="F188">
         <f t="shared" si="4"/>
-        <v>0.83852974784313805</v>
+        <v>0.37088129084967375</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.35">
@@ -4531,11 +4531,11 @@
       </c>
       <c r="E189">
         <f t="shared" si="5"/>
-        <v>2849.237743055558</v>
+        <v>1251.5664444444465</v>
       </c>
       <c r="F189">
         <f t="shared" si="4"/>
-        <v>0.83801110089869357</v>
+        <v>0.36810777777777837</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.35">
@@ -4553,11 +4553,11 @@
       </c>
       <c r="E190">
         <f t="shared" si="5"/>
-        <v>2847.4648195000022</v>
+        <v>1242.136000000002</v>
       </c>
       <c r="F190">
         <f t="shared" si="4"/>
-        <v>0.83748965279411836</v>
+        <v>0.36533411764705942</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.35">
@@ -4575,11 +4575,11 @@
       </c>
       <c r="E191">
         <f t="shared" si="5"/>
-        <v>2845.6824760000022</v>
+        <v>1232.7056111111131</v>
       </c>
       <c r="F191">
         <f t="shared" si="4"/>
-        <v>0.83696543411764768</v>
+        <v>0.36256047385620971</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.35">
@@ -4597,11 +4597,11 @@
       </c>
       <c r="E192">
         <f t="shared" si="5"/>
-        <v>2843.89073377778</v>
+        <v>1223.2753888888908</v>
       </c>
       <c r="F192">
         <f t="shared" si="4"/>
-        <v>0.83643845111111181</v>
+        <v>0.35978687908496787</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.35">
@@ -4619,11 +4619,11 @@
       </c>
       <c r="E193">
         <f t="shared" si="5"/>
-        <v>2842.0896250000023</v>
+        <v>1213.8455000000019</v>
       </c>
       <c r="F193">
         <f t="shared" si="4"/>
-        <v>0.83590871323529481</v>
+        <v>0.35701338235294178</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.35">
@@ -4641,11 +4641,11 @@
       </c>
       <c r="E194">
         <f t="shared" si="5"/>
-        <v>2840.2790383333358</v>
+        <v>1204.415361111113</v>
       </c>
       <c r="F194">
         <f t="shared" si="4"/>
-        <v>0.83537618774509881</v>
+        <v>0.35423981209150385</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.35">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="E195">
         <f t="shared" si="5"/>
-        <v>2838.4591341111136</v>
+        <v>1194.9858055555576</v>
       </c>
       <c r="F195">
         <f t="shared" ref="F195:F258" si="6">E195/3400</f>
-        <v>0.83484092179738634</v>
+        <v>0.35146641339869339</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.35">
@@ -4685,11 +4685,11 @@
       </c>
       <c r="E196">
         <f t="shared" si="5"/>
-        <v>2836.6297464444469</v>
+        <v>1185.5559722222242</v>
       </c>
       <c r="F196">
         <f t="shared" si="6"/>
-        <v>0.83430286660130792</v>
+        <v>0.34869293300653653</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.35">
@@ -4706,12 +4706,12 @@
         <v>-3.3948399999999999</v>
       </c>
       <c r="E197">
-        <f t="shared" ref="E197:E260" si="7">E196+((A197/3600)*D197)</f>
-        <v>2834.7908747777801</v>
+        <f t="shared" ref="E197:E260" si="7">E196+((10/3600)*D197*1000)</f>
+        <v>1176.1258611111132</v>
       </c>
       <c r="F197">
         <f t="shared" si="6"/>
-        <v>0.83376202199346472</v>
+        <v>0.34591937091503328</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.35">
@@ -4729,11 +4729,11 @@
       </c>
       <c r="E198">
         <f t="shared" si="7"/>
-        <v>2832.9426328888912</v>
+        <v>1166.6960555555577</v>
       </c>
       <c r="F198">
         <f t="shared" si="6"/>
-        <v>0.83321842143790914</v>
+        <v>0.34314589869281109</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.35">
@@ -4751,11 +4751,11 @@
       </c>
       <c r="E199">
         <f t="shared" si="7"/>
-        <v>2831.0849283611133</v>
+        <v>1157.2660833333355</v>
       </c>
       <c r="F199">
         <f t="shared" si="6"/>
-        <v>0.83267203775326859</v>
+        <v>0.34037237745098103</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.35">
@@ -4773,11 +4773,11 @@
       </c>
       <c r="E200">
         <f t="shared" si="7"/>
-        <v>2829.2178323611133</v>
+        <v>1147.8363055555576</v>
       </c>
       <c r="F200">
         <f t="shared" si="6"/>
-        <v>0.8321228918709157</v>
+        <v>0.33759891339869341</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.35">
@@ -4795,11 +4795,11 @@
       </c>
       <c r="E201">
         <f t="shared" si="7"/>
-        <v>2827.3413563333356</v>
+        <v>1138.4067777777798</v>
       </c>
       <c r="F201">
         <f t="shared" si="6"/>
-        <v>0.83157098715686339</v>
+        <v>0.33482552287581757</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.35">
@@ -4817,11 +4817,11 @@
       </c>
       <c r="E202">
         <f t="shared" si="7"/>
-        <v>2825.4554007777801</v>
+        <v>1128.9770000000019</v>
       </c>
       <c r="F202">
         <f t="shared" si="6"/>
-        <v>0.83101629434640589</v>
+        <v>0.33205205882352995</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.35">
@@ -4839,11 +4839,11 @@
       </c>
       <c r="E203">
         <f t="shared" si="7"/>
-        <v>2823.5599428611135</v>
+        <v>1119.546861111113</v>
       </c>
       <c r="F203">
         <f t="shared" si="6"/>
-        <v>0.83045880672385697</v>
+        <v>0.32927848856209208</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.35">
@@ -4861,11 +4861,11 @@
       </c>
       <c r="E204">
         <f t="shared" si="7"/>
-        <v>2821.6550435833356</v>
+        <v>1110.1166666666686</v>
       </c>
       <c r="F204">
         <f t="shared" si="6"/>
-        <v>0.82989854223039283</v>
+        <v>0.32650490196078491</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.35">
@@ -4883,11 +4883,11 @@
       </c>
       <c r="E205">
         <f t="shared" si="7"/>
-        <v>2819.7408663611131</v>
+        <v>1100.6872222222241</v>
       </c>
       <c r="F205">
         <f t="shared" si="6"/>
-        <v>0.82933554892973915</v>
+        <v>0.32373153594771298</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.35">
@@ -4905,11 +4905,11 @@
       </c>
       <c r="E206">
         <f t="shared" si="7"/>
-        <v>2817.8170953611129</v>
+        <v>1091.2569722222242</v>
       </c>
       <c r="F206">
         <f t="shared" si="6"/>
-        <v>0.82876973392973907</v>
+        <v>0.32095793300653652</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.35">
@@ -4927,11 +4927,11 @@
       </c>
       <c r="E207">
         <f t="shared" si="7"/>
-        <v>2815.8838542500016</v>
+        <v>1081.8265277777798</v>
       </c>
       <c r="F207">
         <f t="shared" si="6"/>
-        <v>0.82820113360294167</v>
+        <v>0.31818427287581758</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.35">
@@ -4949,11 +4949,11 @@
       </c>
       <c r="E208">
         <f t="shared" si="7"/>
-        <v>2813.9412685277794</v>
+        <v>1072.3965000000021</v>
       </c>
       <c r="F208">
         <f t="shared" si="6"/>
-        <v>0.82762978486111161</v>
+        <v>0.31541073529411828</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.35">
@@ -4971,11 +4971,11 @@
       </c>
       <c r="E209">
         <f t="shared" si="7"/>
-        <v>2811.9892412777795</v>
+        <v>1062.9664166666687</v>
       </c>
       <c r="F209">
         <f t="shared" si="6"/>
-        <v>0.82705565919934687</v>
+        <v>0.31263718137254959</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.35">
@@ -4993,11 +4993,11 @@
       </c>
       <c r="E210">
         <f t="shared" si="7"/>
-        <v>2810.0278186111127</v>
+        <v>1053.536500000002</v>
       </c>
       <c r="F210">
         <f t="shared" si="6"/>
-        <v>0.82647877017973903</v>
+        <v>0.30986367647058882</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.35">
@@ -5015,11 +5015,11 @@
       </c>
       <c r="E211">
         <f t="shared" si="7"/>
-        <v>2808.0568150833351</v>
+        <v>1044.1058611111132</v>
       </c>
       <c r="F211">
         <f t="shared" si="6"/>
-        <v>0.82589906325980444</v>
+        <v>0.30708995915032739</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.35">
@@ -5037,11 +5037,11 @@
       </c>
       <c r="E212">
         <f t="shared" si="7"/>
-        <v>2806.0764450833349</v>
+        <v>1034.67552777778</v>
       </c>
       <c r="F212">
         <f t="shared" si="6"/>
-        <v>0.82531660149509845</v>
+        <v>0.30431633169934702</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.35">
@@ -5059,11 +5059,11 @@
       </c>
       <c r="E213">
         <f t="shared" si="7"/>
-        <v>2804.0866506111129</v>
+        <v>1025.2452222222244</v>
       </c>
       <c r="F213">
         <f t="shared" si="6"/>
-        <v>0.8247313678267979</v>
+        <v>0.30154271241830127</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.35">
@@ -5081,11 +5081,11 @@
       </c>
       <c r="E214">
         <f t="shared" si="7"/>
-        <v>2802.0874493888905</v>
+        <v>1015.81502777778</v>
       </c>
       <c r="F214">
         <f t="shared" si="6"/>
-        <v>0.82414336746732075</v>
+        <v>0.29876912581699411</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.35">
@@ -5103,11 +5103,11 @@
       </c>
       <c r="E215">
         <f t="shared" si="7"/>
-        <v>2800.0789303888905</v>
+        <v>1006.3853611111133</v>
       </c>
       <c r="F215">
         <f t="shared" si="6"/>
-        <v>0.82355262658496775</v>
+        <v>0.29599569444444507</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.35">
@@ -5125,11 +5125,11 @@
       </c>
       <c r="E216">
         <f t="shared" si="7"/>
-        <v>2798.0609876666681</v>
+        <v>996.95572222222438</v>
       </c>
       <c r="F216">
         <f t="shared" si="6"/>
-        <v>0.82295911401960831</v>
+        <v>0.2932222712418307</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.35">
@@ -5147,11 +5147,11 @@
       </c>
       <c r="E217">
         <f t="shared" si="7"/>
-        <v>2796.0335914166681</v>
+        <v>987.52597222222437</v>
       </c>
       <c r="F217">
         <f t="shared" si="6"/>
-        <v>0.82236282100490232</v>
+        <v>0.29044881535947775</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.35">
@@ -5169,11 +5169,11 @@
       </c>
       <c r="E218">
         <f t="shared" si="7"/>
-        <v>2793.9967834166682</v>
+        <v>978.09630555555771</v>
       </c>
       <c r="F218">
         <f t="shared" si="6"/>
-        <v>0.82176375982843186</v>
+        <v>0.28767538398692871</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.35">
@@ -5191,11 +5191,11 @@
       </c>
       <c r="E219">
         <f t="shared" si="7"/>
-        <v>2791.9504372500014</v>
+        <v>968.66613888889106</v>
       </c>
       <c r="F219">
         <f t="shared" si="6"/>
-        <v>0.82116189330882394</v>
+        <v>0.28490180555555622</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.35">
@@ -5213,11 +5213,11 @@
       </c>
       <c r="E220">
         <f t="shared" si="7"/>
-        <v>2789.894812305557</v>
+        <v>959.23666666666884</v>
       </c>
       <c r="F220">
         <f t="shared" si="6"/>
-        <v>0.82055729773692854</v>
+        <v>0.28212843137254967</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.35">
@@ -5235,11 +5235,11 @@
       </c>
       <c r="E221">
         <f t="shared" si="7"/>
-        <v>2787.8296179722238</v>
+        <v>949.80655555555768</v>
       </c>
       <c r="F221">
         <f t="shared" si="6"/>
-        <v>0.81994988763888932</v>
+        <v>0.27935486928104636</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.35">
@@ -5257,11 +5257,11 @@
       </c>
       <c r="E222">
         <f t="shared" si="7"/>
-        <v>2785.7549874166684</v>
+        <v>940.37641666666877</v>
       </c>
       <c r="F222">
         <f t="shared" si="6"/>
-        <v>0.81933970218137309</v>
+        <v>0.27658129901960848</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.35">
@@ -5279,11 +5279,11 @@
       </c>
       <c r="E223">
         <f t="shared" si="7"/>
-        <v>2783.6710188055572</v>
+        <v>930.94669444444651</v>
       </c>
       <c r="F223">
         <f t="shared" si="6"/>
-        <v>0.81872677023692864</v>
+        <v>0.27380785130719015</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.35">
@@ -5301,11 +5301,11 @@
       </c>
       <c r="E224">
         <f t="shared" si="7"/>
-        <v>2781.577749972224</v>
+        <v>921.51755555555758</v>
       </c>
       <c r="F224">
         <f t="shared" si="6"/>
-        <v>0.81811110293300704</v>
+        <v>0.27103457516339929</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.35">
@@ -5323,11 +5323,11 @@
       </c>
       <c r="E225">
         <f t="shared" si="7"/>
-        <v>2779.4749776666686</v>
+        <v>912.08808333333536</v>
       </c>
       <c r="F225">
         <f t="shared" si="6"/>
-        <v>0.81749264049019665</v>
+        <v>0.26826120098039274</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.35">
@@ -5345,11 +5345,11 @@
       </c>
       <c r="E226">
         <f t="shared" si="7"/>
-        <v>2777.3626763333355</v>
+        <v>902.65816666666865</v>
       </c>
       <c r="F226">
         <f t="shared" si="6"/>
-        <v>0.81687137539215748</v>
+        <v>0.26548769607843198</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.35">
@@ -5367,11 +5367,11 @@
       </c>
       <c r="E227">
         <f t="shared" si="7"/>
-        <v>2775.2409638333356</v>
+        <v>893.22833333333529</v>
       </c>
       <c r="F227">
         <f t="shared" si="6"/>
-        <v>0.81624734230392226</v>
+        <v>0.26271421568627507</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.35">
@@ -5389,11 +5389,11 @@
       </c>
       <c r="E228">
         <f t="shared" si="7"/>
-        <v>2773.1097524444467</v>
+        <v>883.79819444444638</v>
       </c>
       <c r="F228">
         <f t="shared" si="6"/>
-        <v>0.81562051542483727</v>
+        <v>0.25994064542483719</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.35">
@@ -5411,11 +5411,11 @@
       </c>
       <c r="E229">
         <f t="shared" si="7"/>
-        <v>2770.9692181111136</v>
+        <v>874.36852777777972</v>
       </c>
       <c r="F229">
         <f t="shared" si="6"/>
-        <v>0.81499094650326875</v>
+        <v>0.25716721405228815</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.35">
@@ -5433,11 +5433,11 @@
       </c>
       <c r="E230">
         <f t="shared" si="7"/>
-        <v>2768.8192857777804</v>
+        <v>864.9390000000019</v>
       </c>
       <c r="F230">
         <f t="shared" si="6"/>
-        <v>0.81435861346405303</v>
+        <v>0.25439382352941231</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.35">
@@ -5455,11 +5455,11 @@
       </c>
       <c r="E231">
         <f t="shared" si="7"/>
-        <v>2766.6598793888916</v>
+        <v>855.50927777777963</v>
       </c>
       <c r="F231">
         <f t="shared" si="6"/>
-        <v>0.81372349393790933</v>
+        <v>0.25162037581699404</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.35">
@@ -5477,11 +5477,11 @@
       </c>
       <c r="E232">
         <f t="shared" si="7"/>
-        <v>2764.4911007777805</v>
+        <v>846.07980555555741</v>
       </c>
       <c r="F232">
         <f t="shared" si="6"/>
-        <v>0.81308561787581779</v>
+        <v>0.24884700163398749</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.35">
@@ -5499,11 +5499,11 @@
       </c>
       <c r="E233">
         <f t="shared" si="7"/>
-        <v>2762.3127322777805</v>
+        <v>836.64963888889076</v>
       </c>
       <c r="F233">
         <f t="shared" si="6"/>
-        <v>0.81244492125817069</v>
+        <v>0.24607342320261494</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.35">
@@ -5521,11 +5521,11 @@
       </c>
       <c r="E234">
         <f t="shared" si="7"/>
-        <v>2760.1250045000029</v>
+        <v>827.21977777777965</v>
       </c>
       <c r="F234">
         <f t="shared" si="6"/>
-        <v>0.81180147191176555</v>
+        <v>0.24329993464052344</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.35">
@@ -5543,11 +5543,11 @@
       </c>
       <c r="E235">
         <f t="shared" si="7"/>
-        <v>2757.9279180555586</v>
+        <v>817.79022222222409</v>
       </c>
       <c r="F235">
         <f t="shared" si="6"/>
-        <v>0.8111552700163408</v>
+        <v>0.24052653594771298</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.35">
@@ -5565,11 +5565,11 @@
       </c>
       <c r="E236">
         <f t="shared" si="7"/>
-        <v>2755.7214020555584</v>
+        <v>808.36066666666852</v>
       </c>
       <c r="F236">
         <f t="shared" si="6"/>
-        <v>0.81050629472222302</v>
+        <v>0.23775313725490252</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.35">
@@ -5587,11 +5587,11 @@
       </c>
       <c r="E237">
         <f t="shared" si="7"/>
-        <v>2753.505417333336</v>
+        <v>798.93094444444625</v>
       </c>
       <c r="F237">
         <f t="shared" si="6"/>
-        <v>0.80985453450980471</v>
+        <v>0.23497968954248419</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.35">
@@ -5609,11 +5609,11 @@
       </c>
       <c r="E238">
         <f t="shared" si="7"/>
-        <v>2751.2800618888914</v>
+        <v>789.50147222222404</v>
       </c>
       <c r="F238">
         <f t="shared" si="6"/>
-        <v>0.80920001820261511</v>
+        <v>0.23220631535947767</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.35">
@@ -5631,11 +5631,11 @@
       </c>
       <c r="E239">
         <f t="shared" si="7"/>
-        <v>2749.0451979722247</v>
+        <v>780.07166666666853</v>
       </c>
       <c r="F239">
         <f t="shared" si="6"/>
-        <v>0.8085427052859484</v>
+        <v>0.22943284313725545</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.35">
@@ -5653,11 +5653,11 @@
       </c>
       <c r="E240">
         <f t="shared" si="7"/>
-        <v>2746.8008910277804</v>
+        <v>770.64180555555743</v>
       </c>
       <c r="F240">
         <f t="shared" si="6"/>
-        <v>0.80788261500817071</v>
+        <v>0.22665935457516395</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.35">
@@ -5675,11 +5675,11 @@
       </c>
       <c r="E241">
         <f t="shared" si="7"/>
-        <v>2744.5471807777803</v>
+        <v>761.21205555555741</v>
       </c>
       <c r="F241">
         <f t="shared" si="6"/>
-        <v>0.80721975905228838</v>
+        <v>0.223885898692811</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.35">
@@ -5697,11 +5697,11 @@
       </c>
       <c r="E242">
         <f t="shared" si="7"/>
-        <v>2742.2839741111138</v>
+        <v>751.7820277777796</v>
       </c>
       <c r="F242">
         <f t="shared" si="6"/>
-        <v>0.80655411003268052</v>
+        <v>0.22111236111111165</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.35">
@@ -5719,11 +5719,11 @@
       </c>
       <c r="E243">
         <f t="shared" si="7"/>
-        <v>2740.0113173333361</v>
+        <v>742.35191666666844</v>
       </c>
       <c r="F243">
         <f t="shared" si="6"/>
-        <v>0.80588568156862828</v>
+        <v>0.21833879901960837</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.35">
@@ -5741,11 +5741,11 @@
       </c>
       <c r="E244">
         <f t="shared" si="7"/>
-        <v>2737.7292909444473</v>
+        <v>732.92205555555734</v>
       </c>
       <c r="F244">
         <f t="shared" si="6"/>
-        <v>0.80521449733660211</v>
+        <v>0.21556531045751687</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.35">
@@ -5763,11 +5763,11 @@
       </c>
       <c r="E245">
         <f t="shared" si="7"/>
-        <v>2735.4378819444473</v>
+        <v>723.49238888889067</v>
       </c>
       <c r="F245">
         <f t="shared" si="6"/>
-        <v>0.80454055351307274</v>
+        <v>0.21279187908496786</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.35">
@@ -5785,11 +5785,11 @@
       </c>
       <c r="E246">
         <f t="shared" si="7"/>
-        <v>2733.1369077222253</v>
+        <v>714.06216666666842</v>
       </c>
       <c r="F246">
         <f t="shared" si="6"/>
-        <v>0.80386379638888983</v>
+        <v>0.21001828431372602</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.35">
@@ -5807,11 +5807,11 @@
       </c>
       <c r="E247">
         <f t="shared" si="7"/>
-        <v>2730.8265781388918</v>
+        <v>704.6322500000017</v>
       </c>
       <c r="F247">
         <f t="shared" si="6"/>
-        <v>0.80318428768790939</v>
+        <v>0.2072447794117652</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.35">
@@ -5829,11 +5829,11 @@
       </c>
       <c r="E248">
         <f t="shared" si="7"/>
-        <v>2728.5067844722253</v>
+        <v>695.20219444444615</v>
       </c>
       <c r="F248">
         <f t="shared" si="6"/>
-        <v>0.80250199543300738</v>
+        <v>0.20447123366013123</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.35">
@@ -5851,11 +5851,11 @@
       </c>
       <c r="E249">
         <f t="shared" si="7"/>
-        <v>2726.1775813333365</v>
+        <v>685.77222222222395</v>
       </c>
       <c r="F249">
         <f t="shared" si="6"/>
-        <v>0.80181693568627543</v>
+        <v>0.20169771241830117</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.35">
@@ -5873,11 +5873,11 @@
       </c>
       <c r="E250">
         <f t="shared" si="7"/>
-        <v>2723.8390928888921</v>
+        <v>676.34283333333508</v>
       </c>
       <c r="F250">
         <f t="shared" si="6"/>
-        <v>0.80112914496732124</v>
+        <v>0.19892436274509856</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.35">
@@ -5895,11 +5895,11 @@
       </c>
       <c r="E251">
         <f t="shared" si="7"/>
-        <v>2721.4909260555587</v>
+        <v>666.91244444444624</v>
       </c>
       <c r="F251">
         <f t="shared" si="6"/>
-        <v>0.80043850766339963</v>
+        <v>0.1961507189542489</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.35">
@@ -5917,11 +5917,11 @@
       </c>
       <c r="E252">
         <f t="shared" si="7"/>
-        <v>2719.133634388892</v>
+        <v>657.48327777777956</v>
       </c>
       <c r="F252">
         <f t="shared" si="6"/>
-        <v>0.79974518658496818</v>
+        <v>0.1933774346405234</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.35">
@@ -5939,11 +5939,11 @@
       </c>
       <c r="E253">
         <f t="shared" si="7"/>
-        <v>2716.7667601666699</v>
+        <v>648.0535000000018</v>
       </c>
       <c r="F253">
         <f t="shared" si="6"/>
-        <v>0.79904904710784408</v>
+        <v>0.19060397058823583</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.35">
@@ -5961,11 +5961,11 @@
       </c>
       <c r="E254">
         <f t="shared" si="7"/>
-        <v>2714.3903301666701</v>
+        <v>638.62322222222406</v>
       </c>
       <c r="F254">
         <f t="shared" si="6"/>
-        <v>0.7983500971078441</v>
+        <v>0.18783035947712473</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.35">
@@ -5983,11 +5983,11 @@
       </c>
       <c r="E255">
         <f t="shared" si="7"/>
-        <v>2712.0045190833366</v>
+        <v>629.19313888889076</v>
       </c>
       <c r="F255">
         <f t="shared" si="6"/>
-        <v>0.79764838796568727</v>
+        <v>0.18505680555555609</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.35">
@@ -6005,11 +6005,11 @@
       </c>
       <c r="E256">
         <f t="shared" si="7"/>
-        <v>2709.6094895833367</v>
+        <v>619.76388888889073</v>
       </c>
       <c r="F256">
         <f t="shared" si="6"/>
-        <v>0.7969439675245108</v>
+        <v>0.18228349673202668</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.35">
@@ -6027,11 +6027,11 @@
       </c>
       <c r="E257">
         <f t="shared" si="7"/>
-        <v>2707.2050025000035</v>
+        <v>610.33452777777961</v>
       </c>
       <c r="F257">
         <f t="shared" si="6"/>
-        <v>0.7962367654411775</v>
+        <v>0.17951015522875871</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.35">
@@ -6049,11 +6049,11 @@
       </c>
       <c r="E258">
         <f t="shared" si="7"/>
-        <v>2704.7911073888922</v>
+        <v>600.90525000000184</v>
       </c>
       <c r="F258">
         <f t="shared" si="6"/>
-        <v>0.79552679629085066</v>
+        <v>0.17673683823529465</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.35">
@@ -6071,11 +6071,11 @@
       </c>
       <c r="E259">
         <f t="shared" si="7"/>
-        <v>2702.3676402222254</v>
+        <v>591.47541666666848</v>
       </c>
       <c r="F259">
         <f t="shared" ref="F259:F321" si="8">E259/3400</f>
-        <v>0.79481401183006628</v>
+        <v>0.17396335784313779</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.35">
@@ -6093,11 +6093,11 @@
       </c>
       <c r="E260">
         <f t="shared" si="7"/>
-        <v>2699.9346787222253</v>
+        <v>582.04533333333518</v>
       </c>
       <c r="F260">
         <f t="shared" si="8"/>
-        <v>0.79409843491830157</v>
+        <v>0.17118980392156918</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.35">
@@ -6114,12 +6114,12 @@
         <v>-3.3947799999999999</v>
       </c>
       <c r="E261">
-        <f t="shared" ref="E261:E321" si="9">E260+((A261/3600)*D261)</f>
-        <v>2697.4923231111143</v>
+        <f t="shared" ref="E261:E321" si="9">E260+((10/3600)*D261*1000)</f>
+        <v>572.61538888889072</v>
       </c>
       <c r="F261">
         <f t="shared" si="8"/>
-        <v>0.7933800950326807</v>
+        <v>0.16841629084967374</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.35">
@@ -6137,11 +6137,11 @@
       </c>
       <c r="E262">
         <f t="shared" si="9"/>
-        <v>2695.0404581111143</v>
+        <v>563.18513888889072</v>
       </c>
       <c r="F262">
         <f t="shared" si="8"/>
-        <v>0.79265895826797483</v>
+        <v>0.16564268790849726</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.35">
@@ -6159,11 +6159,11 @@
       </c>
       <c r="E263">
         <f t="shared" si="9"/>
-        <v>2692.5791918611144</v>
+        <v>553.75500000000181</v>
       </c>
       <c r="F263">
         <f t="shared" si="8"/>
-        <v>0.79193505642973949</v>
+        <v>0.16286911764705936</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.35">
@@ -6181,11 +6181,11 @@
       </c>
       <c r="E264">
         <f t="shared" si="9"/>
-        <v>2690.1086191944478</v>
+        <v>544.32533333333515</v>
       </c>
       <c r="F264">
         <f t="shared" si="8"/>
-        <v>0.7912084174101317</v>
+        <v>0.16009568627451035</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.35">
@@ -6203,11 +6203,11 @@
       </c>
       <c r="E265">
         <f t="shared" si="9"/>
-        <v>2687.6285365000035</v>
+        <v>534.89536111111295</v>
       </c>
       <c r="F265">
         <f t="shared" si="8"/>
-        <v>0.79047898132353045</v>
+        <v>0.15732216503268029</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.35">
@@ -6225,11 +6225,11 @@
       </c>
       <c r="E266">
         <f t="shared" si="9"/>
-        <v>2685.1391118333368</v>
+        <v>525.46572222222403</v>
       </c>
       <c r="F266">
         <f t="shared" si="8"/>
-        <v>0.78974679759804023</v>
+        <v>0.15454874183006589</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.35">
@@ -6247,11 +6247,11 @@
       </c>
       <c r="E267">
         <f t="shared" si="9"/>
-        <v>2682.6403973888923</v>
+        <v>516.03661111111296</v>
       </c>
       <c r="F267">
         <f t="shared" si="8"/>
-        <v>0.78901188158496838</v>
+        <v>0.15177547385620971</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.35">
@@ -6269,11 +6269,11 @@
       </c>
       <c r="E268">
         <f t="shared" si="9"/>
-        <v>2680.1322390555588</v>
+        <v>506.60744444444629</v>
       </c>
       <c r="F268">
         <f t="shared" si="8"/>
-        <v>0.78827418795751725</v>
+        <v>0.1490021895424842</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.35">
@@ -6291,11 +6291,11 @@
       </c>
       <c r="E269">
         <f t="shared" si="9"/>
-        <v>2677.6143993888923</v>
+        <v>497.17733333333518</v>
       </c>
       <c r="F269">
         <f t="shared" si="8"/>
-        <v>0.787533646879086</v>
+        <v>0.14622862745098095</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.35">
@@ -6313,11 +6313,11 @@
       </c>
       <c r="E270">
         <f t="shared" si="9"/>
-        <v>2675.0872189444476</v>
+        <v>487.74755555555743</v>
       </c>
       <c r="F270">
         <f t="shared" si="8"/>
-        <v>0.78679035851307277</v>
+        <v>0.14345516339869335</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.35">
@@ -6335,11 +6335,11 @@
       </c>
       <c r="E271">
         <f t="shared" si="9"/>
-        <v>2672.5506161944477</v>
+        <v>478.31780555555741</v>
       </c>
       <c r="F271">
         <f t="shared" si="8"/>
-        <v>0.78604429888071992</v>
+        <v>0.1406817075163404</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.35">
@@ -6357,11 +6357,11 @@
       </c>
       <c r="E272">
         <f t="shared" si="9"/>
-        <v>2670.0047261944478</v>
+        <v>468.88858333333519</v>
       </c>
       <c r="F272">
         <f t="shared" si="8"/>
-        <v>0.78529550770424938</v>
+        <v>0.13790840686274564</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.35">
@@ -6379,11 +6379,11 @@
       </c>
       <c r="E273">
         <f t="shared" si="9"/>
-        <v>2667.449226305559</v>
+        <v>459.45869444444628</v>
       </c>
       <c r="F273">
         <f t="shared" si="8"/>
-        <v>0.78454389008987035</v>
+        <v>0.13513491013071949</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.35">
@@ -6401,11 +6401,11 @@
       </c>
       <c r="E274">
         <f t="shared" si="9"/>
-        <v>2664.884455194448</v>
+        <v>450.02938888889071</v>
       </c>
       <c r="F274">
         <f t="shared" si="8"/>
-        <v>0.78378954564542591</v>
+        <v>0.13236158496732078</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.35">
@@ -6423,11 +6423,11 @@
       </c>
       <c r="E275">
         <f t="shared" si="9"/>
-        <v>2662.3101106944482</v>
+        <v>440.5995555555574</v>
       </c>
       <c r="F275">
         <f t="shared" si="8"/>
-        <v>0.78303238549836707</v>
+        <v>0.12958810457516395</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.35">
@@ -6445,11 +6445,11 @@
       </c>
       <c r="E276">
         <f t="shared" si="9"/>
-        <v>2659.7264276944484</v>
+        <v>431.17005555555738</v>
       </c>
       <c r="F276">
         <f t="shared" si="8"/>
-        <v>0.78227247873366124</v>
+        <v>0.12681472222222276</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.35">
@@ -6467,11 +6467,11 @@
       </c>
       <c r="E277">
         <f t="shared" si="9"/>
-        <v>2657.133147138893</v>
+        <v>421.73994444444628</v>
       </c>
       <c r="F277">
         <f t="shared" si="8"/>
-        <v>0.78150974915849791</v>
+        <v>0.12404116013071949</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.35">
@@ -6489,11 +6489,11 @@
       </c>
       <c r="E278">
         <f t="shared" si="9"/>
-        <v>2654.5304671388931</v>
+        <v>412.30994444444627</v>
       </c>
       <c r="F278">
         <f t="shared" si="8"/>
-        <v>0.78074425504085088</v>
+        <v>0.12126763071895479</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.35">
@@ -6511,11 +6511,11 @@
       </c>
       <c r="E279">
         <f t="shared" si="9"/>
-        <v>2651.9184263888933</v>
+        <v>402.88019444444626</v>
       </c>
       <c r="F279">
         <f t="shared" si="8"/>
-        <v>0.77997600776143916</v>
+        <v>0.11849417483660184</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.35">
@@ -6533,11 +6533,11 @@
       </c>
       <c r="E280">
         <f t="shared" si="9"/>
-        <v>2649.2970022222266</v>
+        <v>393.45061111111295</v>
       </c>
       <c r="F280">
         <f t="shared" si="8"/>
-        <v>0.7792050006535961</v>
+        <v>0.11572076797385675</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.35">
@@ -6555,11 +6555,11 @@
       </c>
       <c r="E281">
         <f t="shared" si="9"/>
-        <v>2646.6661252222266</v>
+        <v>384.02094444444629</v>
       </c>
       <c r="F281">
         <f t="shared" si="8"/>
-        <v>0.7784312133006549</v>
+        <v>0.11294733660130774</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.35">
@@ -6577,11 +6577,11 @@
       </c>
       <c r="E282">
         <f t="shared" si="9"/>
-        <v>2644.025577444449</v>
+        <v>374.59041666666849</v>
       </c>
       <c r="F282">
         <f t="shared" si="8"/>
-        <v>0.77765458160130851</v>
+        <v>0.11017365196078485</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.35">
@@ -6599,11 +6599,11 @@
       </c>
       <c r="E283">
         <f t="shared" si="9"/>
-        <v>2641.375887944449</v>
+        <v>365.16091666666847</v>
       </c>
       <c r="F283">
         <f t="shared" si="8"/>
-        <v>0.77687526116013206</v>
+        <v>0.10740026960784367</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.35">
@@ -6621,11 +6621,11 @@
       </c>
       <c r="E284">
         <f t="shared" si="9"/>
-        <v>2638.7166279444491</v>
+        <v>355.73091666666846</v>
       </c>
       <c r="F284">
         <f t="shared" si="8"/>
-        <v>0.77609312586601442</v>
+        <v>0.10462674019607895</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.35">
@@ -6643,11 +6643,11 @@
       </c>
       <c r="E285">
         <f t="shared" si="9"/>
-        <v>2636.0479772500048</v>
+        <v>346.30105555555735</v>
       </c>
       <c r="F285">
         <f t="shared" si="8"/>
-        <v>0.77530822860294257</v>
+        <v>0.10185325163398745</v>
       </c>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.35">
@@ -6665,11 +6665,11 @@
       </c>
       <c r="E286">
         <f t="shared" si="9"/>
-        <v>2633.3699361388935</v>
+        <v>336.87133333333514</v>
       </c>
       <c r="F286">
         <f t="shared" si="8"/>
-        <v>0.77452056945261571</v>
+        <v>9.9079803921569162E-2</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.35">
@@ -6687,11 +6687,11 @@
       </c>
       <c r="E287">
         <f t="shared" si="9"/>
-        <v>2630.6824890555604</v>
+        <v>327.44169444444623</v>
       </c>
       <c r="F287">
         <f t="shared" si="8"/>
-        <v>0.77373014383987071</v>
+        <v>9.6306380718954768E-2</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.35">
@@ -6709,11 +6709,11 @@
       </c>
       <c r="E288">
         <f t="shared" si="9"/>
-        <v>2627.985930111116</v>
+        <v>318.01316666666844</v>
       </c>
       <c r="F288">
         <f t="shared" si="8"/>
-        <v>0.77293703826797533</v>
+        <v>9.3533284313726012E-2</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.35">
@@ -6731,11 +6731,11 @@
       </c>
       <c r="E289">
         <f t="shared" si="9"/>
-        <v>2625.2797831944495</v>
+        <v>308.58408333333512</v>
       </c>
       <c r="F289">
         <f t="shared" si="8"/>
-        <v>0.77214111270424979</v>
+        <v>9.0760024509804443E-2</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.35">
@@ -6753,11 +6753,11 @@
       </c>
       <c r="E290">
         <f t="shared" si="9"/>
-        <v>2622.5640711944493</v>
+        <v>299.15452777777955</v>
       </c>
       <c r="F290">
         <f t="shared" si="8"/>
-        <v>0.77134237388072036</v>
+        <v>8.7986625816993985E-2</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.35">
@@ -6775,11 +6775,11 @@
       </c>
       <c r="E291">
         <f t="shared" si="9"/>
-        <v>2619.8390420277829</v>
+        <v>289.72536111111287</v>
       </c>
       <c r="F291">
         <f t="shared" si="8"/>
-        <v>0.77054089471405374</v>
+        <v>8.5213341503268494E-2</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.35">
@@ -6797,11 +6797,11 @@
       </c>
       <c r="E292">
         <f t="shared" si="9"/>
-        <v>2617.1041809166718</v>
+        <v>280.29480555555733</v>
       </c>
       <c r="F292">
         <f t="shared" si="8"/>
-        <v>0.76973652379902113</v>
+        <v>8.243964869281098E-2</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.35">
@@ -6819,11 +6819,11 @@
       </c>
       <c r="E293">
         <f t="shared" si="9"/>
-        <v>2614.3600832500051</v>
+        <v>270.86491666666842</v>
       </c>
       <c r="F293">
         <f t="shared" si="8"/>
-        <v>0.76892943625000154</v>
+        <v>7.9666151960784831E-2</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.35">
@@ -6841,11 +6841,11 @@
       </c>
       <c r="E294">
         <f t="shared" si="9"/>
-        <v>2611.6066124722274</v>
+        <v>261.43522222222396</v>
       </c>
       <c r="F294">
         <f t="shared" si="8"/>
-        <v>0.76811959190359635</v>
+        <v>7.689271241830116E-2</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.35">
@@ -6863,11 +6863,11 @@
       </c>
       <c r="E295">
         <f t="shared" si="9"/>
-        <v>2608.8436550277829</v>
+        <v>252.00533333333507</v>
       </c>
       <c r="F295">
         <f t="shared" si="8"/>
-        <v>0.76730695736111265</v>
+        <v>7.4119215686275025E-2</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.35">
@@ -6885,11 +6885,11 @@
       </c>
       <c r="E296">
         <f t="shared" si="9"/>
-        <v>2606.0713575277828</v>
+        <v>242.57575000000173</v>
       </c>
       <c r="F296">
         <f t="shared" si="8"/>
-        <v>0.76649157574346549</v>
+        <v>7.1345808823529921E-2</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.35">
@@ -6907,11 +6907,11 @@
       </c>
       <c r="E297">
         <f t="shared" si="9"/>
-        <v>2603.2896796111163</v>
+        <v>233.14633333333506</v>
       </c>
       <c r="F297">
         <f t="shared" si="8"/>
-        <v>0.76567343517974007</v>
+        <v>6.8572450980392663E-2</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.35">
@@ -6929,11 +6929,11 @@
       </c>
       <c r="E298">
         <f t="shared" si="9"/>
-        <v>2600.4985969444497</v>
+        <v>223.71700000000175</v>
       </c>
       <c r="F298">
         <f t="shared" si="8"/>
-        <v>0.76485252851307339</v>
+        <v>6.5799117647059341E-2</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.35">
@@ -6951,11 +6951,11 @@
       </c>
       <c r="E299">
         <f t="shared" si="9"/>
-        <v>2597.6981014444495</v>
+        <v>214.28772222222398</v>
       </c>
       <c r="F299">
         <f t="shared" si="8"/>
-        <v>0.76402885336601456</v>
+        <v>6.3025800653595282E-2</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.35">
@@ -6973,11 +6973,11 @@
       </c>
       <c r="E300">
         <f t="shared" si="9"/>
-        <v>2594.8881021666716</v>
+        <v>204.85819444444621</v>
       </c>
       <c r="F300">
         <f t="shared" si="8"/>
-        <v>0.76320238299019749</v>
+        <v>6.0252410130719476E-2</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.35">
@@ -6995,11 +6995,11 @@
       </c>
       <c r="E301">
         <f t="shared" si="9"/>
-        <v>2592.0686484444495</v>
+        <v>195.4285833333351</v>
       </c>
       <c r="F301">
         <f t="shared" si="8"/>
-        <v>0.76237313189542633</v>
+        <v>5.7478995098039734E-2</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.35">
@@ -7017,11 +7017,11 @@
       </c>
       <c r="E302">
         <f t="shared" si="9"/>
-        <v>2589.2395984444497</v>
+        <v>185.99841666666842</v>
       </c>
       <c r="F302">
         <f t="shared" si="8"/>
-        <v>0.7615410583660146</v>
+        <v>5.470541666666718E-2</v>
       </c>
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.35">
@@ -7039,11 +7039,11 @@
       </c>
       <c r="E303">
         <f t="shared" si="9"/>
-        <v>2586.4010346666719</v>
+        <v>176.56797222222397</v>
       </c>
       <c r="F303">
         <f t="shared" si="8"/>
-        <v>0.76070618666666823</v>
+        <v>5.1931756535948226E-2</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.35">
@@ -7061,11 +7061,11 @@
       </c>
       <c r="E304">
         <f t="shared" si="9"/>
-        <v>2583.5533005000052</v>
+        <v>167.13838888889063</v>
       </c>
       <c r="F304">
         <f t="shared" si="8"/>
-        <v>0.75986861779411918</v>
+        <v>4.9158349673203129E-2</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.35">
@@ -7083,11 +7083,11 @@
       </c>
       <c r="E305">
         <f t="shared" si="9"/>
-        <v>2580.6961535833384</v>
+        <v>157.70886111111287</v>
       </c>
       <c r="F305">
         <f t="shared" si="8"/>
-        <v>0.75902828046568771</v>
+        <v>4.6384959150327316E-2</v>
       </c>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.35">
@@ -7105,11 +7105,11 @@
       </c>
       <c r="E306">
         <f t="shared" si="9"/>
-        <v>2577.8293829166719</v>
+        <v>148.27869444444619</v>
       </c>
       <c r="F306">
         <f t="shared" si="8"/>
-        <v>0.75818511262255051</v>
+        <v>4.3611380718954762E-2</v>
       </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.35">
@@ -7127,11 +7127,11 @@
       </c>
       <c r="E307">
         <f t="shared" si="9"/>
-        <v>2574.9532583333385</v>
+        <v>138.84877777777953</v>
       </c>
       <c r="F307">
         <f t="shared" si="8"/>
-        <v>0.7573391936274525</v>
+        <v>4.0837875816993982E-2</v>
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.35">
@@ -7149,11 +7149,11 @@
       </c>
       <c r="E308">
         <f t="shared" si="9"/>
-        <v>2572.0678313333383</v>
+        <v>129.41927777777954</v>
       </c>
       <c r="F308">
         <f t="shared" si="8"/>
-        <v>0.75649053862745241</v>
+        <v>3.8064493464052808E-2</v>
       </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.35">
@@ -7171,11 +7171,11 @@
       </c>
       <c r="E309">
         <f t="shared" si="9"/>
-        <v>2569.1729407222274</v>
+        <v>119.98966666666843</v>
       </c>
       <c r="F309">
         <f t="shared" si="8"/>
-        <v>0.75563910021241987</v>
+        <v>3.5291078431373066E-2</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.35">
@@ -7193,11 +7193,11 @@
       </c>
       <c r="E310">
         <f t="shared" si="9"/>
-        <v>2566.2684408333384</v>
+        <v>110.55947222222399</v>
       </c>
       <c r="F310">
         <f t="shared" si="8"/>
-        <v>0.75478483553921716</v>
+        <v>3.251749183006588E-2</v>
       </c>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.35">
@@ -7215,11 +7215,11 @@
       </c>
       <c r="E311">
         <f t="shared" si="9"/>
-        <v>2563.3545107500049</v>
+        <v>101.12927777777955</v>
       </c>
       <c r="F311">
         <f t="shared" si="8"/>
-        <v>0.75392779727941317</v>
+        <v>2.974390522875869E-2</v>
       </c>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.35">
@@ -7237,11 +7237,11 @@
       </c>
       <c r="E312">
         <f t="shared" si="9"/>
-        <v>2560.4312538055606</v>
+        <v>91.699416666668441</v>
       </c>
       <c r="F312">
         <f t="shared" si="8"/>
-        <v>0.75306801582516492</v>
+        <v>2.6970416666667187E-2</v>
       </c>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.35">
@@ -7259,11 +7259,11 @@
       </c>
       <c r="E313">
         <f t="shared" si="9"/>
-        <v>2557.498558361116</v>
+        <v>82.269527777779558</v>
       </c>
       <c r="F313">
         <f t="shared" si="8"/>
-        <v>0.75220545834150476</v>
+        <v>2.4196919934641046E-2</v>
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.35">
@@ -7281,11 +7281,11 @@
       </c>
       <c r="E314">
         <f t="shared" si="9"/>
-        <v>2554.5565370277827</v>
+        <v>72.839972222224006</v>
       </c>
       <c r="F314">
         <f t="shared" si="8"/>
-        <v>0.75134015794934783</v>
+        <v>2.1423521241830591E-2</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.35">
@@ -7303,11 +7303,11 @@
       </c>
       <c r="E315">
         <f t="shared" si="9"/>
-        <v>2551.6050426666716</v>
+        <v>63.410277777779562</v>
       </c>
       <c r="F315">
         <f t="shared" si="8"/>
-        <v>0.75047207137255045</v>
+        <v>1.865008169934693E-2</v>
       </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.35">
@@ -7325,11 +7325,11 @@
       </c>
       <c r="E316">
         <f t="shared" si="9"/>
-        <v>2548.6440662777827</v>
+        <v>53.980416666668454</v>
       </c>
       <c r="F316">
         <f t="shared" si="8"/>
-        <v>0.74960119596405372</v>
+        <v>1.5876593137255427E-2</v>
       </c>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.35">
@@ -7347,11 +7347,11 @@
       </c>
       <c r="E317">
         <f t="shared" si="9"/>
-        <v>2545.6738875277829</v>
+        <v>44.551277777779568</v>
       </c>
       <c r="F317">
         <f t="shared" si="8"/>
-        <v>0.74872761397875964</v>
+        <v>1.3103316993464578E-2</v>
       </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.35">
@@ -7369,11 +7369,11 @@
       </c>
       <c r="E318">
         <f t="shared" si="9"/>
-        <v>2542.6942796388939</v>
+        <v>35.122138888890682</v>
       </c>
       <c r="F318">
         <f t="shared" si="8"/>
-        <v>0.74785125871732172</v>
+        <v>1.0330040849673729E-2</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.35">
@@ -7391,11 +7391,11 @@
       </c>
       <c r="E319">
         <f t="shared" si="9"/>
-        <v>2539.7051721666717</v>
+        <v>25.692777777779572</v>
       </c>
       <c r="F319">
         <f t="shared" si="8"/>
-        <v>0.74697210946078574</v>
+        <v>7.5566993464057566E-3</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.35">
@@ -7413,11 +7413,11 @@
       </c>
       <c r="E320">
         <f t="shared" si="9"/>
-        <v>2536.7064675000051</v>
+        <v>16.262888888890682</v>
       </c>
       <c r="F320">
         <f t="shared" si="8"/>
-        <v>0.74609013750000153</v>
+        <v>4.7832026143796126E-3</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.35">
@@ -7435,11 +7435,11 @@
       </c>
       <c r="E321">
         <f t="shared" si="9"/>
-        <v>2533.6984126944494</v>
+        <v>6.8332500000017919</v>
       </c>
       <c r="F321">
         <f t="shared" si="8"/>
-        <v>0.7452054154983675</v>
+        <v>2.0097794117652328E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>